<commit_message>
Added line numbers, rule, and few edits on review comments
</commit_message>
<xml_diff>
--- a/CodeReviewResults.xlsx
+++ b/CodeReviewResults.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="127">
   <si>
     <t xml:space="preserve">File </t>
   </si>
@@ -142,15 +142,6 @@
     INF_Bin [NC_MD_239] = 0;
     strncpy( SUF_Bin,(const char*) &amp;BEnreg[unFileEndingIndex], NC_MD_239 );
     SUF_Bin [NC_MD_239] = 0;</t>
-  </si>
-  <si>
-    <t>Sprecis &amp; Iprecis return values should be RANGE verified before we them as buffer offsets.</t>
-  </si>
-  <si>
-    <t>IPrecis = strlenw( INF_Bin, NC_MD_239, ' ' );
-    SPrecis = strlenw( SUF_Bin, NC_MD_239, ' ' );
-    memset( &amp;INF_Bin[IPrecis], '0', NC_MD_239 - IPrecis );
-    memset( &amp;SUF_Bin[SPrecis], '9', NC_MD_239 - SPrecis );</t>
   </si>
   <si>
     <t>if ( IsoBuf[0] == START_SENTINELLE )
@@ -251,9 +242,6 @@
 function.</t>
   </si>
   <si>
-    <t>TMP_CodeCredit_CheckServiceCode</t>
-  </si>
-  <si>
     <t>for(unIndexCodeService = 0; unIndexCodeService &lt; NC_MD_287 ; unIndexCodeService++)</t>
   </si>
   <si>
@@ -271,9 +259,6 @@
     <t>return statement missing for the function</t>
   </si>
   <si>
-    <t>TMP_CodeCredit_GetSameNumber</t>
-  </si>
-  <si>
     <t>int TMP_CodeCredit_GetSameNumber( unsigned char *pDataToCheck, 
 unsigned char * pCurrentEnreg, unsigned short unFileBeginningIndex,
  unsigned short unTailleMax)</t>
@@ -296,9 +281,6 @@
  }</t>
   </si>
   <si>
-    <t>Init</t>
-  </si>
-  <si>
     <t>strncpy (m_szOutputFilePath, pszOutputFilePath, MAX_PATH);</t>
   </si>
   <si>
@@ -323,29 +305,12 @@
     <t>Init (const char *pszOutputFilePath, const char *pszPublicKeyFilePath, bool fOutputBase64Only)</t>
   </si>
   <si>
-    <t>(m_cbWrittenHeader == 0)
-Use NULL for clarity
-(m_cbWrittenHeader == NULL)</t>
-  </si>
-  <si>
     <t>char szHexIV[32] = {0};
         StrnDevHexa (szHexIV, (char*)m_bufIV, 16);
         szHexIV[32] = 0;</t>
   </si>
   <si>
-    <t>WriteData</t>
-  </si>
-  <si>
     <t>(1 != EVP_EncryptUpdate (&amp;m_evtCipherContext, m_bufCipheredDataForBase64+m_cbAvailableForBase64, &amp;cbCiphered, m_bufClearDataForAES, cbReadyToAesCipher))</t>
-  </si>
-  <si>
-    <t>m_bufBase64output should be checked for NULL</t>
-  </si>
-  <si>
-    <t>m_cbWrittenBase64 += fwrite (m_bufBase64output, 1, cbBase64, m_pfTmpOutputFile);</t>
-  </si>
-  <si>
-    <t>This function is heavily depending on Class variables cannot say whether it is OK or not as do not know the context</t>
   </si>
   <si>
     <t>#ifdef LOG_ALL
@@ -357,9 +322,6 @@
     <t>Remove commented code</t>
   </si>
   <si>
-    <t>memcpy(tmptrc, m_bufClearDataForAES, cbReadyToAesCipher];</t>
-  </si>
-  <si>
     <t>tmptrc[cbReadyToAesCipher] = 0;</t>
   </si>
   <si>
@@ -390,12 +352,6 @@
     <t>CodeReview1.cpp
 TMP_CodeCredit_CheckPANInsideBINs
 26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INCORRECT LENGTH passed.
-sizeof(IsoBuf) gives length of pointer.
-Use sizeof(PanValue)
-</t>
   </si>
   <si>
     <t>Use pre-increment to avoid calling constructor every time</t>
@@ -470,12 +426,234 @@
     <t>Heap overflow
 tmptrc[cbReadyToAesCipher] = 0;</t>
   </si>
+  <si>
+    <t>error</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp</t>
+  </si>
+  <si>
+    <t>Invalid number of character &amp;amp;#039;[&amp;amp;#039; when no macros are defined." verbose="Invalid number of character &amp;amp;#039;[&amp;amp;#039; when no macros are defined.</t>
+  </si>
+  <si>
+    <t>Invalid number of character &amp;amp;#039;[&amp;amp;#039; when these macros are defined: &amp;amp;#039;LOG_ALL&amp;amp;#039;." verbose="Invalid number of character &amp;amp;#039;[&amp;amp;#039; when these macros are defined: &amp;amp;#039;LOG_ALL&amp;amp;#039;.</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+WriteData</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+TMP_CodeCredit_CheckPANInsideBINs
+38</t>
+  </si>
+  <si>
+    <t>Passing buffer Index(es) as part function parameters is NOT reccomended. Address passing should be handled by the caller function.
+Also, use sizeof() for length to ensure fewer modifications in case where we change the buffer size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INCORRECT LENGTH passed.
+sizeof(IsoBuf) gives length of pointer.
+Use sizeof(PanValue) - 1 with strncpy function if IsoBuf is expected to be NULL terminated
+If NOT Caller must pass the length
+</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+TMP_CodeCredit_CheckPANInsideBINs
+52</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+TMP_CodeCredit_CheckPANInsideBINs
+58</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+TMP_CodeCredit_CheckPANInsideBINs
+65</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+TMP_CodeCredit_CheckPANInsideBINs
+70, 77</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+TMP_CodeCredit_CheckPANInsideBINs
+70</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+TMP_CodeCredit_CheckPANInsideBINs
+82</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+TMP_CodeCredit_CheckPANInsideBINs
+109</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+TMP_CodeCredit_CheckPANInsideBINs
+121</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+TMP_CodeCredit_CheckServiceCode
+130</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+TMP_CodeCredit_CheckServiceCode
+159</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+TMP_CodeCredit_CheckServiceCode
+238</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+TMP_CodeCredit_GetSameNumber
+257</t>
+  </si>
+  <si>
+    <t>acInfPlage NOT initialized</t>
+  </si>
+  <si>
+    <t>char acInfPlage[NC_MD_239]; //NC_MD_239 est la plus grande taille Ã  regarder</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+TMP_CodeCredit_GetSameNumber
+261</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+TMP_CodeCredit_GetSameNumber
+264</t>
+  </si>
+  <si>
+    <t>strncpy( acInfPlage,(const char*) &amp;pCurrentEnreg[unFileBeginningIndex], unTailleMax );</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+TMP_CodeCredit_GetSameNumber
+267</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+Init
+345</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+Init
+370</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+Init
+363</t>
+  </si>
+  <si>
+    <t>FileUtils::GetTempFilePath (pszOutputFilePath, true, "VF_", m_szTmpOutputFilePath, MAX_PATH);</t>
+  </si>
+  <si>
+    <t>Use sizeof() for length</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+Init
+339</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+Init
+423</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+WriteData
+507</t>
+  </si>
+  <si>
+    <t>data should be checked for NULL</t>
+  </si>
+  <si>
+    <t>bool SecuredFileWriter::WriteData (const char *data, size_t len)</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+WriteData
+452</t>
+  </si>
+  <si>
+    <t>This function is heavily depending on Class variables cannot say whether it is OK or not, as do not know the context</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+Finalize
+597</t>
+  </si>
+  <si>
+    <r>
+      <t>memcpy(tmptrc, m_bufClearDataForAES, cbReadyToAesCipher</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>];</t>
+    </r>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+Finalize
+598</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+Finalize
+604</t>
+  </si>
+  <si>
+    <t>tmptrc should be checked for NULL</t>
+  </si>
+  <si>
+    <t>char* tmptrc = new char[cbReadyToAesCipher];
+            memcpy(tmptrc, m_bufClearDataForAES, cbReadyToAesCipher];</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+Finalize
+596</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+Finalize
+649</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+Finalize
+664</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+Finalize
+666</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -525,6 +703,12 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -688,7 +872,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -717,9 +901,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -778,7 +959,79 @@
     <cellStyle name="Excel_BuiltIn_Heading 1" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="69">
+  <dxfs count="77">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1828,7 +2081,7 @@
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.33203125" customWidth="1"/>
-    <col min="2" max="2" width="27.33203125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" style="17" customWidth="1"/>
     <col min="3" max="3" width="42.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.5546875" customWidth="1"/>
@@ -1858,11 +2111,11 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="19">
+      <c r="A2" s="18">
         <v>43091</v>
       </c>
-      <c r="B2" s="17" t="s">
-        <v>80</v>
+      <c r="B2" s="16" t="s">
+        <v>69</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5" t="s">
@@ -1878,7 +2131,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
-      <c r="B3" s="17"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -1888,7 +2141,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
-      <c r="B4" s="17"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -1901,7 +2154,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
-      <c r="B5" s="17"/>
+      <c r="B5" s="16"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -1914,7 +2167,7 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
-      <c r="B6" s="17"/>
+      <c r="B6" s="16"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -1924,7 +2177,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
-      <c r="B7" s="17"/>
+      <c r="B7" s="16"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -1934,7 +2187,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
-      <c r="B8" s="17"/>
+      <c r="B8" s="16"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
@@ -1944,7 +2197,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
-      <c r="B9" s="17"/>
+      <c r="B9" s="16"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
@@ -1954,7 +2207,7 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
-      <c r="B10" s="17"/>
+      <c r="B10" s="16"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -1964,7 +2217,7 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
-      <c r="B11" s="17"/>
+      <c r="B11" s="16"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -1974,7 +2227,7 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
-      <c r="B12" s="17"/>
+      <c r="B12" s="16"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -1984,7 +2237,7 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
-      <c r="B13" s="17"/>
+      <c r="B13" s="16"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
@@ -1994,147 +2247,147 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
-      <c r="B14" s="17"/>
+      <c r="B14" s="16"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
-      <c r="B15" s="17"/>
+      <c r="B15" s="16"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
-      <c r="B16" s="17"/>
+      <c r="B16" s="16"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
-      <c r="B17" s="17"/>
+      <c r="B17" s="16"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
-      <c r="B18" s="17"/>
+      <c r="B18" s="16"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
-      <c r="B19" s="17"/>
+      <c r="B19" s="16"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
-      <c r="B20" s="17"/>
+      <c r="B20" s="16"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
-      <c r="B21" s="17"/>
+      <c r="B21" s="16"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
-      <c r="B22" s="17"/>
+      <c r="B22" s="16"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
-      <c r="B23" s="17"/>
+      <c r="B23" s="16"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
-      <c r="B24" s="17"/>
+      <c r="B24" s="16"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
-      <c r="B25" s="17"/>
+      <c r="B25" s="16"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
-      <c r="B26" s="17"/>
+      <c r="B26" s="16"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
-      <c r="B27" s="17"/>
+      <c r="B27" s="16"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
-      <c r="B28" s="17"/>
+      <c r="B28" s="16"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
-      <c r="B29" s="17"/>
+      <c r="B29" s="16"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
-      <c r="B30" s="17"/>
+      <c r="B30" s="16"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
-      <c r="B31" s="17"/>
+      <c r="B31" s="16"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
-      <c r="B32" s="17"/>
+      <c r="B32" s="16"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
-      <c r="B33" s="17"/>
+      <c r="B33" s="16"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
-      <c r="B34" s="17"/>
+      <c r="B34" s="16"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
@@ -2173,18 +2426,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:D34">
-    <cfRule type="cellIs" dxfId="68" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="3" stopIfTrue="1" operator="equal">
       <formula>$Q$2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="4" stopIfTrue="1" operator="equal">
       <formula>$Q$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E34">
-    <cfRule type="cellIs" dxfId="66" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="1" stopIfTrue="1" operator="equal">
       <formula>$Q$2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="2" stopIfTrue="1" operator="equal">
       <formula>$Q$1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2200,20 +2453,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="46" customWidth="1"/>
-    <col min="2" max="2" width="40.88671875" customWidth="1"/>
+    <col min="2" max="2" width="40.88671875" style="15" customWidth="1"/>
     <col min="3" max="3" width="61.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="80.77734375" style="37" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="80.77734375" style="36" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.44140625" customWidth="1"/>
-    <col min="6" max="6" width="19.88671875" style="14" customWidth="1"/>
+    <col min="6" max="6" width="19.88671875" style="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2226,7 +2479,7 @@
       <c r="C1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="33" t="s">
         <v>24</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -2236,437 +2489,592 @@
     </row>
     <row r="2" spans="1:6" ht="227.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="B2" s="16"/>
+        <v>71</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>15</v>
+      </c>
       <c r="C2" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="D2" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="15" t="s">
         <v>27</v>
       </c>
       <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:6" ht="227.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
+      <c r="A3" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>19</v>
+      </c>
       <c r="C3" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="15" t="s">
         <v>27</v>
       </c>
       <c r="F3" s="10"/>
     </row>
     <row r="4" spans="1:6" ht="227.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
+      <c r="A4" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>22</v>
+      </c>
       <c r="C4" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="E4" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="10"/>
+    </row>
+    <row r="5" spans="1:6" ht="81.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="11"/>
+    </row>
+    <row r="6" spans="1:6" ht="86.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E6" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="10"/>
-    </row>
-    <row r="5" spans="1:6" ht="227.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="D5" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="10"/>
-    </row>
-    <row r="6" spans="1:6" ht="81.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="11"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="D6" s="35" t="s">
-        <v>85</v>
-      </c>
-      <c r="E6" s="16" t="s">
+      <c r="F6" s="12"/>
+    </row>
+    <row r="7" spans="1:6" ht="111.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="11"/>
-    </row>
-    <row r="7" spans="1:6" ht="86.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="11"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="35" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="12"/>
-    </row>
-    <row r="8" spans="1:6" ht="111.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
-      <c r="B8" s="16"/>
+      <c r="F7" s="10"/>
+    </row>
+    <row r="8" spans="1:6" ht="227.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>10</v>
+      </c>
       <c r="C8" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="D8" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="10"/>
+    </row>
+    <row r="9" spans="1:6" ht="134.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E9" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="10"/>
-    </row>
-    <row r="9" spans="1:6" ht="227.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="16" t="s">
+      <c r="F9" s="10"/>
+    </row>
+    <row r="10" spans="1:6" ht="134.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="10"/>
-    </row>
-    <row r="10" spans="1:6" ht="134.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16" t="s">
+      <c r="F10" s="10"/>
+    </row>
+    <row r="11" spans="1:6" ht="134.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" s="16" t="s">
+      <c r="D11" s="34"/>
+      <c r="E11" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="10"/>
-    </row>
-    <row r="11" spans="1:6" ht="134.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="15"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="35" t="s">
+      <c r="F11" s="10"/>
+    </row>
+    <row r="12" spans="1:6" ht="134.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E12" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="10"/>
-    </row>
-    <row r="12" spans="1:6" ht="134.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="15"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="11" t="s">
+      <c r="F12" s="10"/>
+    </row>
+    <row r="13" spans="1:6" ht="134.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="35"/>
-      <c r="E12" s="16" t="s">
+      <c r="E13" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="10"/>
+    </row>
+    <row r="14" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="35"/>
+      <c r="E14" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F12" s="10"/>
-    </row>
-    <row r="13" spans="1:6" ht="134.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="D13" s="35" t="s">
+    </row>
+    <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D15" s="36" t="s">
+        <v>100</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="10"/>
+    </row>
+    <row r="16" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E16" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="10"/>
-    </row>
-    <row r="14" spans="1:6" ht="134.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="15"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="D14" s="35" t="s">
+    </row>
+    <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E17" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" s="36" t="s">
+        <v>103</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="F14" s="10"/>
-    </row>
-    <row r="15" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="13"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="36"/>
-      <c r="E15" s="16" t="s">
+    </row>
+    <row r="20" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A20" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F16" s="10"/>
-    </row>
-    <row r="17" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="37" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17" s="16" t="s">
+    <row r="21" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" s="15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C18" s="33" t="s">
-        <v>84</v>
-      </c>
-      <c r="D18" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="E18" s="16" t="s">
+    <row r="22" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22" s="15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="C19" s="33" t="s">
-        <v>87</v>
-      </c>
-      <c r="E19" s="16" t="s">
+    <row r="23" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" s="15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="C20" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="E20" s="16" t="s">
+    <row r="24" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A24" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="D22" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="E22" s="16" t="s">
+    <row r="26" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="E26" s="15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C23" s="33" t="s">
+    <row r="27" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A27" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" t="s">
+        <v>113</v>
+      </c>
+      <c r="D27" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A29" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A31" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="D31" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A32" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="D23" s="37" t="s">
-        <v>60</v>
-      </c>
-      <c r="E23" s="16" t="s">
+      <c r="E32" s="15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C24" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="D24" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="E24" s="16" t="s">
+    <row r="33" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A33" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" t="s">
+        <v>121</v>
+      </c>
+      <c r="D33" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="E33" s="15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C25" s="33" t="s">
+    <row r="34" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A34" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" t="s">
+        <v>64</v>
+      </c>
+      <c r="D34" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A35" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="E25" s="16" t="s">
+      <c r="D35" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="E35" s="15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="C26" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="D26" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="E26" s="16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>65</v>
-      </c>
-      <c r="C28" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="D28" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="E28" s="16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C29" t="s">
+    <row r="36" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A36" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" t="s">
         <v>67</v>
       </c>
-      <c r="D29" s="37" t="s">
+      <c r="D36" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="E29" s="16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C30" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="E30" s="16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="C31" t="s">
-        <v>71</v>
-      </c>
-      <c r="D31" s="37" t="s">
-        <v>70</v>
-      </c>
-      <c r="E31" s="16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C32" s="33" t="s">
-        <v>89</v>
-      </c>
-      <c r="D32" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="E32" s="16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="33" spans="3:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C33" s="33" t="s">
-        <v>90</v>
-      </c>
-      <c r="D33" s="37" t="s">
-        <v>73</v>
-      </c>
-      <c r="E33" s="16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="34" spans="3:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C34" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="D34" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="E34" s="16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="35" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C35" t="s">
-        <v>67</v>
-      </c>
-      <c r="D35" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="E35" s="16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="36" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C36" t="s">
-        <v>75</v>
-      </c>
-      <c r="D36" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="E36" s="16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="37" spans="3:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C37" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="D37" s="37" t="s">
-        <v>77</v>
-      </c>
-      <c r="E37" s="16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="38" spans="3:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C38" t="s">
-        <v>78</v>
-      </c>
-      <c r="D38" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="E38" s="16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="39" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C39" t="s">
-        <v>67</v>
-      </c>
-      <c r="D39" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="E39" s="16" t="s">
+      <c r="E36" s="15" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B26:B36 B2:B24">
       <formula1>Rules</formula1>
     </dataValidation>
   </dataValidations>
@@ -2676,7 +3084,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="61" stopIfTrue="1" operator="equal" id="{4DA63688-A84B-41FA-A0E8-0582C6C2B836}">
+          <x14:cfRule type="cellIs" priority="65" stopIfTrue="1" operator="equal" id="{4DA63688-A84B-41FA-A0E8-0582C6C2B836}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -2686,7 +3094,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="62" stopIfTrue="1" operator="equal" id="{E3AD87B5-E648-44C6-88B0-11F945431B87}">
+          <x14:cfRule type="cellIs" priority="66" stopIfTrue="1" operator="equal" id="{E3AD87B5-E648-44C6-88B0-11F945431B87}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -2700,10 +3108,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E4 E6:E8 E10 E16 E21 E27 E40:E61</xm:sqref>
+          <xm:sqref>E5:E7 E9 E25 E37:E58</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="59" stopIfTrue="1" operator="equal" id="{602A14BB-9BDF-4C1A-812D-6A0EB6747D9F}">
+          <x14:cfRule type="cellIs" priority="63" stopIfTrue="1" operator="equal" id="{602A14BB-9BDF-4C1A-812D-6A0EB6747D9F}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -2713,7 +3121,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="60" stopIfTrue="1" operator="equal" id="{02AA9148-8E20-4F32-980D-8B224188FA80}">
+          <x14:cfRule type="cellIs" priority="64" stopIfTrue="1" operator="equal" id="{02AA9148-8E20-4F32-980D-8B224188FA80}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -2730,7 +3138,7 @@
           <xm:sqref>E3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="57" stopIfTrue="1" operator="equal" id="{8C5A4143-3864-49CB-86A9-B0F33F284F6A}">
+          <x14:cfRule type="cellIs" priority="61" stopIfTrue="1" operator="equal" id="{8C5A4143-3864-49CB-86A9-B0F33F284F6A}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -2740,7 +3148,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="58" stopIfTrue="1" operator="equal" id="{9D149001-F424-4461-9604-446FFDB08447}">
+          <x14:cfRule type="cellIs" priority="62" stopIfTrue="1" operator="equal" id="{9D149001-F424-4461-9604-446FFDB08447}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -2757,7 +3165,7 @@
           <xm:sqref>E2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="55" stopIfTrue="1" operator="equal" id="{9F8BFDA5-8974-4E40-94C6-1D81EE086C93}">
+          <x14:cfRule type="cellIs" priority="59" stopIfTrue="1" operator="equal" id="{9F8BFDA5-8974-4E40-94C6-1D81EE086C93}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -2767,7 +3175,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="56" stopIfTrue="1" operator="equal" id="{EB6EE14A-7FC5-460A-A34B-4EBF8872ABC0}">
+          <x14:cfRule type="cellIs" priority="60" stopIfTrue="1" operator="equal" id="{EB6EE14A-7FC5-460A-A34B-4EBF8872ABC0}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -2781,10 +3189,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E5</xm:sqref>
+          <xm:sqref>E4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="53" stopIfTrue="1" operator="equal" id="{94A6B6BB-4DDE-4209-B1AA-4070E24FA1BF}">
+          <x14:cfRule type="cellIs" priority="57" stopIfTrue="1" operator="equal" id="{94A6B6BB-4DDE-4209-B1AA-4070E24FA1BF}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -2794,7 +3202,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="54" stopIfTrue="1" operator="equal" id="{ED5E38E6-3983-43A4-8574-3950052808E6}">
+          <x14:cfRule type="cellIs" priority="58" stopIfTrue="1" operator="equal" id="{ED5E38E6-3983-43A4-8574-3950052808E6}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -2808,10 +3216,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E9</xm:sqref>
+          <xm:sqref>E8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="51" stopIfTrue="1" operator="equal" id="{E9316EA5-6F05-40B4-A750-5EEF9C6F8A31}">
+          <x14:cfRule type="cellIs" priority="55" stopIfTrue="1" operator="equal" id="{E9316EA5-6F05-40B4-A750-5EEF9C6F8A31}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -2821,7 +3229,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="52" stopIfTrue="1" operator="equal" id="{E84C1040-9433-4D42-99E8-7182A05B5257}">
+          <x14:cfRule type="cellIs" priority="56" stopIfTrue="1" operator="equal" id="{E84C1040-9433-4D42-99E8-7182A05B5257}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -2835,10 +3243,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E11</xm:sqref>
+          <xm:sqref>E10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="49" stopIfTrue="1" operator="equal" id="{85C59230-A024-4095-B166-305386F38BD8}">
+          <x14:cfRule type="cellIs" priority="53" stopIfTrue="1" operator="equal" id="{85C59230-A024-4095-B166-305386F38BD8}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -2848,7 +3256,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="50" stopIfTrue="1" operator="equal" id="{6BDC9A61-D471-4FC3-B9A1-CD84A5C6A728}">
+          <x14:cfRule type="cellIs" priority="54" stopIfTrue="1" operator="equal" id="{6BDC9A61-D471-4FC3-B9A1-CD84A5C6A728}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -2862,10 +3270,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E12</xm:sqref>
+          <xm:sqref>E11</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="47" stopIfTrue="1" operator="equal" id="{C1A10AEC-D27E-497B-86D5-140AEFADD175}">
+          <x14:cfRule type="cellIs" priority="51" stopIfTrue="1" operator="equal" id="{C1A10AEC-D27E-497B-86D5-140AEFADD175}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -2875,7 +3283,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="48" stopIfTrue="1" operator="equal" id="{EFA23895-A9FB-44B9-99C7-BE8530108E75}">
+          <x14:cfRule type="cellIs" priority="52" stopIfTrue="1" operator="equal" id="{EFA23895-A9FB-44B9-99C7-BE8530108E75}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -2889,10 +3297,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E13</xm:sqref>
+          <xm:sqref>E12</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="45" stopIfTrue="1" operator="equal" id="{A4551ED4-8FB8-4495-830B-4AFDD0CBC3D5}">
+          <x14:cfRule type="cellIs" priority="49" stopIfTrue="1" operator="equal" id="{A4551ED4-8FB8-4495-830B-4AFDD0CBC3D5}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -2902,7 +3310,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="46" stopIfTrue="1" operator="equal" id="{11CF0586-45AE-4C3B-B577-2F64BA9254EE}">
+          <x14:cfRule type="cellIs" priority="50" stopIfTrue="1" operator="equal" id="{11CF0586-45AE-4C3B-B577-2F64BA9254EE}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -2916,10 +3324,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E14</xm:sqref>
+          <xm:sqref>E13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="43" stopIfTrue="1" operator="equal" id="{AB48A264-90BF-4883-9FA6-004AB47A8687}">
+          <x14:cfRule type="cellIs" priority="47" stopIfTrue="1" operator="equal" id="{AB48A264-90BF-4883-9FA6-004AB47A8687}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -2929,7 +3337,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="44" stopIfTrue="1" operator="equal" id="{272F72DD-4D07-43E5-A783-D375CED1401A}">
+          <x14:cfRule type="cellIs" priority="48" stopIfTrue="1" operator="equal" id="{272F72DD-4D07-43E5-A783-D375CED1401A}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -2943,10 +3351,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E15</xm:sqref>
+          <xm:sqref>E14</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="41" stopIfTrue="1" operator="equal" id="{6CF7CF66-F40A-4BF2-989A-F0A9EA1207C0}">
+          <x14:cfRule type="cellIs" priority="45" stopIfTrue="1" operator="equal" id="{6CF7CF66-F40A-4BF2-989A-F0A9EA1207C0}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -2956,7 +3364,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="42" stopIfTrue="1" operator="equal" id="{E77CDF33-4731-4BD2-B67D-45CDA616F6FB}">
+          <x14:cfRule type="cellIs" priority="46" stopIfTrue="1" operator="equal" id="{E77CDF33-4731-4BD2-B67D-45CDA616F6FB}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -2970,10 +3378,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E17</xm:sqref>
+          <xm:sqref>E16</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="39" stopIfTrue="1" operator="equal" id="{723D429E-2271-49E4-BABA-ED32592ADEA1}">
+          <x14:cfRule type="cellIs" priority="43" stopIfTrue="1" operator="equal" id="{723D429E-2271-49E4-BABA-ED32592ADEA1}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -2983,7 +3391,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="40" stopIfTrue="1" operator="equal" id="{6BDAAC76-3BF4-4342-A8CB-AEC648647476}">
+          <x14:cfRule type="cellIs" priority="44" stopIfTrue="1" operator="equal" id="{6BDAAC76-3BF4-4342-A8CB-AEC648647476}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -2997,10 +3405,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E18</xm:sqref>
+          <xm:sqref>E17</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="37" stopIfTrue="1" operator="equal" id="{0A5A250E-298D-45D2-B4F7-1AA08E820D92}">
+          <x14:cfRule type="cellIs" priority="41" stopIfTrue="1" operator="equal" id="{0A5A250E-298D-45D2-B4F7-1AA08E820D92}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -3010,7 +3418,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="38" stopIfTrue="1" operator="equal" id="{F65669EA-7A7F-456F-B6F9-AE11248E28A5}">
+          <x14:cfRule type="cellIs" priority="42" stopIfTrue="1" operator="equal" id="{F65669EA-7A7F-456F-B6F9-AE11248E28A5}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -3024,10 +3432,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E19</xm:sqref>
+          <xm:sqref>E18</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="35" stopIfTrue="1" operator="equal" id="{509068B4-3D5A-4625-A659-7B7771383D1D}">
+          <x14:cfRule type="cellIs" priority="39" stopIfTrue="1" operator="equal" id="{509068B4-3D5A-4625-A659-7B7771383D1D}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -3037,7 +3445,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="36" stopIfTrue="1" operator="equal" id="{19B27BBC-893E-4B04-A6E1-E94ED1B39028}">
+          <x14:cfRule type="cellIs" priority="40" stopIfTrue="1" operator="equal" id="{19B27BBC-893E-4B04-A6E1-E94ED1B39028}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -3051,10 +3459,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E20</xm:sqref>
+          <xm:sqref>E19</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="33" stopIfTrue="1" operator="equal" id="{1806BF15-7656-4D02-891F-C2C88F533618}">
+          <x14:cfRule type="cellIs" priority="37" stopIfTrue="1" operator="equal" id="{1806BF15-7656-4D02-891F-C2C88F533618}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -3064,7 +3472,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="34" stopIfTrue="1" operator="equal" id="{4EDE58C4-F656-4887-AD66-7C45E0C9F154}">
+          <x14:cfRule type="cellIs" priority="38" stopIfTrue="1" operator="equal" id="{4EDE58C4-F656-4887-AD66-7C45E0C9F154}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -3078,10 +3486,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E22</xm:sqref>
+          <xm:sqref>E20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="31" stopIfTrue="1" operator="equal" id="{603A0457-A83C-4696-81AE-C6601F79E859}">
+          <x14:cfRule type="cellIs" priority="35" stopIfTrue="1" operator="equal" id="{603A0457-A83C-4696-81AE-C6601F79E859}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -3091,7 +3499,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="32" stopIfTrue="1" operator="equal" id="{96ACD1D5-1D77-44D3-A870-F3C509AA1619}">
+          <x14:cfRule type="cellIs" priority="36" stopIfTrue="1" operator="equal" id="{96ACD1D5-1D77-44D3-A870-F3C509AA1619}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -3105,10 +3513,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E23</xm:sqref>
+          <xm:sqref>E21</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="29" stopIfTrue="1" operator="equal" id="{42E9A256-6C7C-4981-B010-4099E20FABCA}">
+          <x14:cfRule type="cellIs" priority="33" stopIfTrue="1" operator="equal" id="{42E9A256-6C7C-4981-B010-4099E20FABCA}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -3118,7 +3526,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="30" stopIfTrue="1" operator="equal" id="{2CB1E213-6AEA-4B1A-AB01-53AAD0D5790F}">
+          <x14:cfRule type="cellIs" priority="34" stopIfTrue="1" operator="equal" id="{2CB1E213-6AEA-4B1A-AB01-53AAD0D5790F}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -3132,10 +3540,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E24</xm:sqref>
+          <xm:sqref>E23</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="27" stopIfTrue="1" operator="equal" id="{2BB8ECB4-B458-431F-8B6F-A9D66DCA866C}">
+          <x14:cfRule type="cellIs" priority="29" stopIfTrue="1" operator="equal" id="{57CC6C1A-4D4E-49B6-832C-89A45E88CFE7}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -3145,7 +3553,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="28" stopIfTrue="1" operator="equal" id="{9929C749-EC47-4FCA-B877-0A9DC451736A}">
+          <x14:cfRule type="cellIs" priority="30" stopIfTrue="1" operator="equal" id="{315E6B91-235A-445B-B517-F9C5B1D37EAE}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -3159,10 +3567,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E25</xm:sqref>
+          <xm:sqref>E24</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="25" stopIfTrue="1" operator="equal" id="{57CC6C1A-4D4E-49B6-832C-89A45E88CFE7}">
+          <x14:cfRule type="cellIs" priority="27" stopIfTrue="1" operator="equal" id="{4B1E35FF-0116-4119-9C46-B62114BCB4D1}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -3172,7 +3580,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="26" stopIfTrue="1" operator="equal" id="{315E6B91-235A-445B-B517-F9C5B1D37EAE}">
+          <x14:cfRule type="cellIs" priority="28" stopIfTrue="1" operator="equal" id="{1BEF4AE7-FF76-48FD-815B-DF262AE3CFE0}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -3189,7 +3597,7 @@
           <xm:sqref>E26</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="23" stopIfTrue="1" operator="equal" id="{4B1E35FF-0116-4119-9C46-B62114BCB4D1}">
+          <x14:cfRule type="cellIs" priority="25" stopIfTrue="1" operator="equal" id="{56A818B0-64D8-4601-90CC-C6EDD507EA9C}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -3199,7 +3607,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="24" stopIfTrue="1" operator="equal" id="{1BEF4AE7-FF76-48FD-815B-DF262AE3CFE0}">
+          <x14:cfRule type="cellIs" priority="26" stopIfTrue="1" operator="equal" id="{17B3CA77-595F-408E-BE76-D589997E775B}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -3213,10 +3621,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E28</xm:sqref>
+          <xm:sqref>E27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="21" stopIfTrue="1" operator="equal" id="{56A818B0-64D8-4601-90CC-C6EDD507EA9C}">
+          <x14:cfRule type="cellIs" priority="23" stopIfTrue="1" operator="equal" id="{8EFB9414-826C-4022-A42F-DBF2E2ACBD12}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -3226,7 +3634,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="22" stopIfTrue="1" operator="equal" id="{17B3CA77-595F-408E-BE76-D589997E775B}">
+          <x14:cfRule type="cellIs" priority="24" stopIfTrue="1" operator="equal" id="{37CA990F-0EB9-4F54-968D-AF772C0F3C2F}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -3240,10 +3648,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E29</xm:sqref>
+          <xm:sqref>E28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="19" stopIfTrue="1" operator="equal" id="{8EFB9414-826C-4022-A42F-DBF2E2ACBD12}">
+          <x14:cfRule type="cellIs" priority="21" stopIfTrue="1" operator="equal" id="{51379761-3831-4490-968E-247ABD1A188C}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -3253,7 +3661,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="20" stopIfTrue="1" operator="equal" id="{37CA990F-0EB9-4F54-968D-AF772C0F3C2F}">
+          <x14:cfRule type="cellIs" priority="22" stopIfTrue="1" operator="equal" id="{71DA6DDA-5280-4ADC-A4F0-C4A726FF5E8A}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -3267,10 +3675,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E30</xm:sqref>
+          <xm:sqref>E29</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="17" stopIfTrue="1" operator="equal" id="{51379761-3831-4490-968E-247ABD1A188C}">
+          <x14:cfRule type="cellIs" priority="19" stopIfTrue="1" operator="equal" id="{7000E78B-8344-4F21-8566-805BB092F3D8}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -3280,7 +3688,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="18" stopIfTrue="1" operator="equal" id="{71DA6DDA-5280-4ADC-A4F0-C4A726FF5E8A}">
+          <x14:cfRule type="cellIs" priority="20" stopIfTrue="1" operator="equal" id="{3F33EA94-08A9-4DCF-BEC6-E70B2D7DC02D}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -3294,10 +3702,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E31</xm:sqref>
+          <xm:sqref>E30</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="15" stopIfTrue="1" operator="equal" id="{7000E78B-8344-4F21-8566-805BB092F3D8}">
+          <x14:cfRule type="cellIs" priority="17" stopIfTrue="1" operator="equal" id="{9A282710-C433-496A-A098-FAD9D4C6A268}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -3307,7 +3715,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="16" stopIfTrue="1" operator="equal" id="{3F33EA94-08A9-4DCF-BEC6-E70B2D7DC02D}">
+          <x14:cfRule type="cellIs" priority="18" stopIfTrue="1" operator="equal" id="{D6811E4F-319E-4C10-8B82-9D4173AF56A0}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -3321,10 +3729,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E32</xm:sqref>
+          <xm:sqref>E31</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="13" stopIfTrue="1" operator="equal" id="{9A282710-C433-496A-A098-FAD9D4C6A268}">
+          <x14:cfRule type="cellIs" priority="15" stopIfTrue="1" operator="equal" id="{56B58C0B-73C7-45C7-880B-A8A864AEEB5F}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -3334,7 +3742,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="14" stopIfTrue="1" operator="equal" id="{D6811E4F-319E-4C10-8B82-9D4173AF56A0}">
+          <x14:cfRule type="cellIs" priority="16" stopIfTrue="1" operator="equal" id="{7F7F6FA1-0D19-4448-8002-D9882A8ABA6C}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -3348,10 +3756,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E33</xm:sqref>
+          <xm:sqref>E32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="11" stopIfTrue="1" operator="equal" id="{56B58C0B-73C7-45C7-880B-A8A864AEEB5F}">
+          <x14:cfRule type="cellIs" priority="13" stopIfTrue="1" operator="equal" id="{F8759862-0F30-4D84-AAFA-113B17483CFF}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -3361,7 +3769,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="12" stopIfTrue="1" operator="equal" id="{7F7F6FA1-0D19-4448-8002-D9882A8ABA6C}">
+          <x14:cfRule type="cellIs" priority="14" stopIfTrue="1" operator="equal" id="{E858A037-4BA5-410C-B670-8D7A8C222E96}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -3375,10 +3783,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E34</xm:sqref>
+          <xm:sqref>E33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="9" stopIfTrue="1" operator="equal" id="{F8759862-0F30-4D84-AAFA-113B17483CFF}">
+          <x14:cfRule type="cellIs" priority="11" stopIfTrue="1" operator="equal" id="{74263FAC-CF77-4538-BBD8-73F2C08179CC}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -3388,7 +3796,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="10" stopIfTrue="1" operator="equal" id="{E858A037-4BA5-410C-B670-8D7A8C222E96}">
+          <x14:cfRule type="cellIs" priority="12" stopIfTrue="1" operator="equal" id="{A3DD3372-D965-4C24-85A4-EA6E4382C7D6}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -3402,10 +3810,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E35</xm:sqref>
+          <xm:sqref>E34</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="7" stopIfTrue="1" operator="equal" id="{74263FAC-CF77-4538-BBD8-73F2C08179CC}">
+          <x14:cfRule type="cellIs" priority="9" stopIfTrue="1" operator="equal" id="{BC224CCD-AED0-47E8-A807-BC68B81EBB46}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -3415,7 +3823,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="8" stopIfTrue="1" operator="equal" id="{A3DD3372-D965-4C24-85A4-EA6E4382C7D6}">
+          <x14:cfRule type="cellIs" priority="10" stopIfTrue="1" operator="equal" id="{13CDBA54-459C-429C-976B-B6B80CF25615}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -3429,10 +3837,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E36</xm:sqref>
+          <xm:sqref>E35</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="5" stopIfTrue="1" operator="equal" id="{BC224CCD-AED0-47E8-A807-BC68B81EBB46}">
+          <x14:cfRule type="cellIs" priority="7" stopIfTrue="1" operator="equal" id="{FA246ABD-99D2-48A5-B712-63D5DE1373BB}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -3442,7 +3850,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="6" stopIfTrue="1" operator="equal" id="{13CDBA54-459C-429C-976B-B6B80CF25615}">
+          <x14:cfRule type="cellIs" priority="8" stopIfTrue="1" operator="equal" id="{ACD219FD-8B2C-4CEC-B767-5D010594E27A}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -3456,10 +3864,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E37</xm:sqref>
+          <xm:sqref>E36</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="3" stopIfTrue="1" operator="equal" id="{FA246ABD-99D2-48A5-B712-63D5DE1373BB}">
+          <x14:cfRule type="cellIs" priority="3" stopIfTrue="1" operator="equal" id="{527FF2D0-730F-4E2D-BB75-072DDE5D9BC0}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -3469,7 +3877,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="4" stopIfTrue="1" operator="equal" id="{ACD219FD-8B2C-4CEC-B767-5D010594E27A}">
+          <x14:cfRule type="cellIs" priority="4" stopIfTrue="1" operator="equal" id="{A6CFC000-223C-4E5D-9B15-371B831ADF9F}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -3483,10 +3891,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E38</xm:sqref>
+          <xm:sqref>E22</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="1" stopIfTrue="1" operator="equal" id="{8717F435-7F80-476D-92BB-A9364D2D94DA}">
+          <x14:cfRule type="cellIs" priority="1" stopIfTrue="1" operator="equal" id="{77049A23-0BD6-4761-A28E-A3AA974475F7}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -3496,7 +3904,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="2" stopIfTrue="1" operator="equal" id="{DD5C3359-E926-4745-AEAC-400F171FAB86}">
+          <x14:cfRule type="cellIs" priority="2" stopIfTrue="1" operator="equal" id="{4462B2BB-D1CC-4F36-B92C-4D660C855A60}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -3510,7 +3918,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E39</xm:sqref>
+          <xm:sqref>E15</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -3520,7 +3928,7 @@
           <x14:formula1>
             <xm:f>History!$Q$4:$Q$5</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E15 E17:E20 E22:E26 E28:E39</xm:sqref>
+          <xm:sqref>E26:E36 E2:E24</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3533,15 +3941,15 @@
   <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="71.6640625" customWidth="1"/>
+    <col min="4" max="4" width="212.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -3559,369 +3967,385 @@
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="20"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="22"/>
-    </row>
-    <row r="3" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="23"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="25"/>
-    </row>
-    <row r="4" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="23"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="25"/>
-    </row>
-    <row r="5" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="23"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="22"/>
-    </row>
-    <row r="6" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="23"/>
-      <c r="B6" s="31"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="26"/>
-    </row>
-    <row r="7" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="23"/>
-      <c r="B7" s="31"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="26"/>
-    </row>
-    <row r="8" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="23"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="25"/>
-    </row>
-    <row r="9" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="23"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="25"/>
-    </row>
-    <row r="10" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="23"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="25"/>
-    </row>
-    <row r="11" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="23"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="25"/>
-    </row>
-    <row r="12" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="23"/>
-      <c r="B12" s="31"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="25"/>
-    </row>
-    <row r="13" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="23"/>
-      <c r="B13" s="31"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="26"/>
-    </row>
-    <row r="14" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="23"/>
-      <c r="B14" s="31"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="26"/>
-    </row>
-    <row r="15" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="23"/>
-      <c r="B15" s="31"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="26"/>
-    </row>
-    <row r="16" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="23"/>
-      <c r="B16" s="31"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="26"/>
-    </row>
-    <row r="17" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="23"/>
-      <c r="B17" s="31"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="26"/>
-    </row>
-    <row r="18" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="23"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="26"/>
-    </row>
-    <row r="19" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="23"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="26"/>
-    </row>
-    <row r="20" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="23"/>
-      <c r="B20" s="31"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="26"/>
-    </row>
-    <row r="21" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="23"/>
-      <c r="B21" s="31"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="26"/>
-    </row>
-    <row r="22" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="23"/>
-      <c r="B22" s="31"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="26"/>
-    </row>
-    <row r="23" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="23"/>
-      <c r="B23" s="31"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="26"/>
-    </row>
-    <row r="24" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="23"/>
-      <c r="B24" s="31"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="26"/>
-    </row>
-    <row r="25" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="23"/>
-      <c r="B25" s="31"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="26"/>
-    </row>
-    <row r="26" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="23"/>
-      <c r="B26" s="31"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="26"/>
-    </row>
-    <row r="27" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="23"/>
-      <c r="B27" s="31"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="26"/>
-    </row>
-    <row r="28" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="23"/>
-      <c r="B28" s="31"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="26"/>
-    </row>
-    <row r="29" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="23"/>
-      <c r="B29" s="31"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="26"/>
-    </row>
-    <row r="30" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="23"/>
-      <c r="B30" s="31"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="26"/>
-    </row>
-    <row r="31" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="23"/>
-      <c r="B31" s="31"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="26"/>
-    </row>
-    <row r="32" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="23"/>
-      <c r="B32" s="31"/>
-      <c r="C32" s="24"/>
-      <c r="D32" s="26"/>
-    </row>
-    <row r="33" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="23"/>
-      <c r="B33" s="31"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="26"/>
-    </row>
-    <row r="34" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="23"/>
-      <c r="B34" s="31"/>
-      <c r="C34" s="24"/>
-      <c r="D34" s="26"/>
-    </row>
-    <row r="35" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="23"/>
-      <c r="B35" s="31"/>
-      <c r="C35" s="24"/>
-      <c r="D35" s="26"/>
-    </row>
-    <row r="36" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="23"/>
-      <c r="B36" s="31"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="25"/>
-    </row>
-    <row r="37" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="23"/>
-      <c r="B37" s="31"/>
-      <c r="C37" s="24"/>
-      <c r="D37" s="26"/>
-    </row>
-    <row r="38" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="23"/>
-      <c r="B38" s="31"/>
-      <c r="C38" s="24"/>
-      <c r="D38" s="26"/>
-    </row>
-    <row r="39" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="23"/>
-      <c r="B39" s="31"/>
-      <c r="C39" s="24"/>
-      <c r="D39" s="26"/>
-    </row>
-    <row r="40" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="23"/>
-      <c r="B40" s="31"/>
-      <c r="C40" s="24"/>
-      <c r="D40" s="26"/>
-    </row>
-    <row r="41" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="23"/>
-      <c r="B41" s="31"/>
-      <c r="C41" s="24"/>
-      <c r="D41" s="26"/>
-    </row>
-    <row r="42" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="23"/>
-      <c r="B42" s="31"/>
-      <c r="C42" s="24"/>
-      <c r="D42" s="26"/>
-    </row>
-    <row r="43" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="23"/>
-      <c r="B43" s="31"/>
-      <c r="C43" s="24"/>
-      <c r="D43" s="26"/>
-    </row>
-    <row r="44" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="23"/>
-      <c r="B44" s="31"/>
-      <c r="C44" s="24"/>
-      <c r="D44" s="26"/>
-    </row>
-    <row r="45" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="23"/>
-      <c r="B45" s="31"/>
-      <c r="C45" s="24"/>
-      <c r="D45" s="26"/>
-    </row>
-    <row r="46" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="23"/>
-      <c r="B46" s="31"/>
-      <c r="C46" s="24"/>
-      <c r="D46" s="25"/>
-    </row>
-    <row r="47" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="23"/>
-      <c r="B47" s="31"/>
-      <c r="C47" s="24"/>
-      <c r="D47" s="26"/>
-    </row>
-    <row r="48" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="23"/>
-      <c r="B48" s="31"/>
-      <c r="C48" s="24"/>
-      <c r="D48" s="26"/>
-    </row>
-    <row r="49" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="23"/>
-      <c r="B49" s="31"/>
-      <c r="C49" s="24"/>
-      <c r="D49" s="26"/>
-    </row>
-    <row r="50" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="23"/>
-      <c r="B50" s="31"/>
-      <c r="C50" s="24"/>
-      <c r="D50" s="26"/>
-    </row>
-    <row r="51" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="23"/>
-      <c r="B51" s="31"/>
-      <c r="C51" s="24"/>
-      <c r="D51" s="26"/>
-    </row>
-    <row r="52" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="23"/>
-      <c r="B52" s="31"/>
-      <c r="C52" s="24"/>
-      <c r="D52" s="26"/>
-    </row>
-    <row r="53" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="23"/>
-      <c r="B53" s="31"/>
-      <c r="C53" s="24"/>
-      <c r="D53" s="26"/>
-    </row>
-    <row r="54" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="27"/>
-      <c r="B54" s="32"/>
-      <c r="C54" s="28"/>
-      <c r="D54" s="29"/>
-    </row>
-    <row r="55" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="20">
+        <v>597</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="20">
+        <v>597</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="22"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="24"/>
+    </row>
+    <row r="5" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="22"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="21"/>
+    </row>
+    <row r="6" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="22"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="25"/>
+    </row>
+    <row r="7" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="22"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="25"/>
+    </row>
+    <row r="8" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="22"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="24"/>
+    </row>
+    <row r="9" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="22"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="24"/>
+    </row>
+    <row r="10" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="22"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="24"/>
+    </row>
+    <row r="11" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="22"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="24"/>
+    </row>
+    <row r="12" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="22"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="24"/>
+    </row>
+    <row r="13" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="22"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="25"/>
+    </row>
+    <row r="14" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="22"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="25"/>
+    </row>
+    <row r="15" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="22"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="25"/>
+    </row>
+    <row r="16" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="22"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="25"/>
+    </row>
+    <row r="17" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="22"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="25"/>
+    </row>
+    <row r="18" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="22"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="25"/>
+    </row>
+    <row r="19" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="22"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="25"/>
+    </row>
+    <row r="20" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="22"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="25"/>
+    </row>
+    <row r="21" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="22"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="25"/>
+    </row>
+    <row r="22" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="22"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="25"/>
+    </row>
+    <row r="23" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="22"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="25"/>
+    </row>
+    <row r="24" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="22"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="25"/>
+    </row>
+    <row r="25" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="22"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="25"/>
+    </row>
+    <row r="26" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="22"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="25"/>
+    </row>
+    <row r="27" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="22"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="25"/>
+    </row>
+    <row r="28" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="22"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="25"/>
+    </row>
+    <row r="29" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="22"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="25"/>
+    </row>
+    <row r="30" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="22"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="25"/>
+    </row>
+    <row r="31" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="22"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="25"/>
+    </row>
+    <row r="32" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="22"/>
+      <c r="B32" s="30"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="25"/>
+    </row>
+    <row r="33" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="22"/>
+      <c r="B33" s="30"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="25"/>
+    </row>
+    <row r="34" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="22"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="25"/>
+    </row>
+    <row r="35" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="22"/>
+      <c r="B35" s="30"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="25"/>
+    </row>
+    <row r="36" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="22"/>
+      <c r="B36" s="30"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="24"/>
+    </row>
+    <row r="37" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="22"/>
+      <c r="B37" s="30"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="25"/>
+    </row>
+    <row r="38" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="22"/>
+      <c r="B38" s="30"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="25"/>
+    </row>
+    <row r="39" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="22"/>
+      <c r="B39" s="30"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="25"/>
+    </row>
+    <row r="40" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="22"/>
+      <c r="B40" s="30"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="25"/>
+    </row>
+    <row r="41" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="22"/>
+      <c r="B41" s="30"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="25"/>
+    </row>
+    <row r="42" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="22"/>
+      <c r="B42" s="30"/>
+      <c r="C42" s="23"/>
+      <c r="D42" s="25"/>
+    </row>
+    <row r="43" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="22"/>
+      <c r="B43" s="30"/>
+      <c r="C43" s="23"/>
+      <c r="D43" s="25"/>
+    </row>
+    <row r="44" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="22"/>
+      <c r="B44" s="30"/>
+      <c r="C44" s="23"/>
+      <c r="D44" s="25"/>
+    </row>
+    <row r="45" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="22"/>
+      <c r="B45" s="30"/>
+      <c r="C45" s="23"/>
+      <c r="D45" s="25"/>
+    </row>
+    <row r="46" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="22"/>
+      <c r="B46" s="30"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="24"/>
+    </row>
+    <row r="47" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="22"/>
+      <c r="B47" s="30"/>
+      <c r="C47" s="23"/>
+      <c r="D47" s="25"/>
+    </row>
+    <row r="48" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="22"/>
+      <c r="B48" s="30"/>
+      <c r="C48" s="23"/>
+      <c r="D48" s="25"/>
+    </row>
+    <row r="49" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="22"/>
+      <c r="B49" s="30"/>
+      <c r="C49" s="23"/>
+      <c r="D49" s="25"/>
+    </row>
+    <row r="50" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="22"/>
+      <c r="B50" s="30"/>
+      <c r="C50" s="23"/>
+      <c r="D50" s="25"/>
+    </row>
+    <row r="51" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="22"/>
+      <c r="B51" s="30"/>
+      <c r="C51" s="23"/>
+      <c r="D51" s="25"/>
+    </row>
+    <row r="52" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="22"/>
+      <c r="B52" s="30"/>
+      <c r="C52" s="23"/>
+      <c r="D52" s="25"/>
+    </row>
+    <row r="53" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="22"/>
+      <c r="B53" s="30"/>
+      <c r="C53" s="23"/>
+      <c r="D53" s="25"/>
+    </row>
+    <row r="54" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="26"/>
+      <c r="B54" s="31"/>
+      <c r="C54" s="27"/>
+      <c r="D54" s="28"/>
+    </row>
+    <row r="55" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="12"/>
     </row>
-    <row r="56" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="12"/>
     </row>
-    <row r="57" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="12"/>
     </row>
-    <row r="58" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="12"/>
     </row>
-    <row r="59" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="12"/>
     </row>
-    <row r="60" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="12"/>
     </row>
-    <row r="61" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="12"/>
     </row>
-    <row r="62" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="12"/>
     </row>
-    <row r="63" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="12"/>
     </row>
-    <row r="64" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="12"/>
     </row>
-    <row r="65" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="12"/>
     </row>
-    <row r="66" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="12"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>"WARNING"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
       <formula>"Style"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
       <formula>"ERROR"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Couple of new finding before final commit
</commit_message>
<xml_diff>
--- a/CodeReviewResults.xlsx
+++ b/CodeReviewResults.xlsx
@@ -17,6 +17,7 @@
     <sheet name="CPP_Check" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Manual_Review!$E$1:$E$39</definedName>
     <definedName name="Rules">History!$R$1:$R$13</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="142">
   <si>
     <t xml:space="preserve">File </t>
   </si>
@@ -155,13 +156,6 @@
     }</t>
   </si>
   <si>
-    <t>Use of memcmp reccomended</t>
-  </si>
-  <si>
-    <t>strlen( PanValue )
-Calculate string length once and use everywhere unless the PanValue is altered</t>
-  </si>
-  <si>
     <t>//On padde le Pan avec des 00 pour indiquer le dÃ©but de la plage carte
     memset( INC_Bin, '0', NC_MD_239 );
     memcpy( INC_Bin, PanValue, strlen( PanValue ) );
@@ -170,52 +164,6 @@
     memset( SUC_Bin, '9', NC_MD_239 );
  memcpy( SUC_Bin, PanValue, strlen( PanValue ) );
  SUC_Bin[NC_MD_239] = 0;</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Easy Method</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-memset( INC_Bin, '0', NC_MD_239 );
-    memcpy( INC_Bin, PanValue, strlen( PanValue ) );
-    INC_Bin[NC_MD_239] = 0;
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>A better one:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-panLen=strlen( PanValue );
-memcpy( INC_Bin, PanValue,  panLen);
-memcpy( &amp;INC_Bin[panLen], '0',  NC_MD_239 - panLen);
-    INC_Bin[NC_MD_239] = 0;</t>
-    </r>
   </si>
   <si>
     <t>if (( strcmp( INC_Bin, INF_Bin ) &gt;= 0 ) &amp;&amp; ( strcmp( SUF_Bin, SUC_Bin ) &gt;= 0 ) ) 
@@ -267,9 +215,6 @@
     <t>for(indexPlage = 0; indexPlage &lt; MAX(unTailleMax,NC_MD_239); indexPlage++)</t>
   </si>
   <si>
-    <t>BUFFER OVERFLOW</t>
-  </si>
-  <si>
     <t>for(indexPlage = 0; indexPlage &lt; MAX(unTailleMax,NC_MD_239); indexPlage++)
  {
   //Tant que la donnÃ©e est Ã©quivalente jusqu'Ã  la limite, alors on continue la comparaison
@@ -284,11 +229,6 @@
     <t>strncpy (m_szOutputFilePath, pszOutputFilePath, MAX_PATH);</t>
   </si>
   <si>
-    <t>Use sizeof() if (m_szOutputFilePath is a static buffer
-strncpy (m_szOutputFilePath, pszOutputFilePath, sizeof((m_szOutputFilePath));
-if m_szOutputFilePath is a pointer, must pass size of buffer as parameter and use as max length</t>
-  </si>
-  <si>
     <t>Be UNIFORM with indentation of conditions
 (1 != EVP_EncryptInit_ex (&amp;m_evtCipherContext, EVP_aes_256_cbc(), NULL, m_bufAesKey, m_bufIV))</t>
   </si>
@@ -300,9 +240,6 @@
 pszOutputFilePath
 pszPublicKeyFilePath
 </t>
-  </si>
-  <si>
-    <t>Init (const char *pszOutputFilePath, const char *pszPublicKeyFilePath, bool fOutputBase64Only)</t>
   </si>
   <si>
     <t>char szHexIV[32] = {0};
@@ -386,6 +323,529 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">
+szHexIV[32] = 0; is a OVERFLOW
+Buffer size should be 32 + 1
+char szHexIV[32 + 1] = {0};</t>
+  </si>
+  <si>
+    <t>un-compiled code? :-)
+Really unexpected !!!</t>
+  </si>
+  <si>
+    <t>Heap overflow
+tmptrc[cbReadyToAesCipher] = 0;</t>
+  </si>
+  <si>
+    <t>error</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp</t>
+  </si>
+  <si>
+    <t>Invalid number of character &amp;amp;#039;[&amp;amp;#039; when no macros are defined." verbose="Invalid number of character &amp;amp;#039;[&amp;amp;#039; when no macros are defined.</t>
+  </si>
+  <si>
+    <t>Invalid number of character &amp;amp;#039;[&amp;amp;#039; when these macros are defined: &amp;amp;#039;LOG_ALL&amp;amp;#039;." verbose="Invalid number of character &amp;amp;#039;[&amp;amp;#039; when these macros are defined: &amp;amp;#039;LOG_ALL&amp;amp;#039;.</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+WriteData</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+TMP_CodeCredit_CheckPANInsideBINs
+38</t>
+  </si>
+  <si>
+    <t>Passing buffer Index(es) as part function parameters is NOT reccomended. Address passing should be handled by the caller function.
+Also, use sizeof() for length to ensure fewer modifications in case where we change the buffer size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INCORRECT LENGTH passed.
+sizeof(IsoBuf) gives length of pointer.
+Use sizeof(PanValue) - 1 with strncpy function if IsoBuf is expected to be NULL terminated
+If NOT Caller must pass the length
+</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+TMP_CodeCredit_CheckPANInsideBINs
+52</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+TMP_CodeCredit_CheckPANInsideBINs
+58</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+TMP_CodeCredit_CheckPANInsideBINs
+65</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+TMP_CodeCredit_CheckPANInsideBINs
+70, 77</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+TMP_CodeCredit_CheckPANInsideBINs
+70</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+TMP_CodeCredit_CheckPANInsideBINs
+82</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+TMP_CodeCredit_CheckServiceCode
+130</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+TMP_CodeCredit_CheckServiceCode
+159</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+TMP_CodeCredit_CheckServiceCode
+238</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+TMP_CodeCredit_GetSameNumber
+257</t>
+  </si>
+  <si>
+    <t>acInfPlage NOT initialized</t>
+  </si>
+  <si>
+    <t>char acInfPlage[NC_MD_239]; //NC_MD_239 est la plus grande taille Ã  regarder</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+TMP_CodeCredit_GetSameNumber
+261</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+TMP_CodeCredit_GetSameNumber
+264</t>
+  </si>
+  <si>
+    <t>strncpy( acInfPlage,(const char*) &amp;pCurrentEnreg[unFileBeginningIndex], unTailleMax );</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+TMP_CodeCredit_GetSameNumber
+267</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+Init
+345</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+Init
+370</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+Init
+363</t>
+  </si>
+  <si>
+    <t>FileUtils::GetTempFilePath (pszOutputFilePath, true, "VF_", m_szTmpOutputFilePath, MAX_PATH);</t>
+  </si>
+  <si>
+    <t>Use sizeof() for length</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+Init
+339</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+Init
+423</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+WriteData
+507</t>
+  </si>
+  <si>
+    <t>data should be checked for NULL</t>
+  </si>
+  <si>
+    <t>bool SecuredFileWriter::WriteData (const char *data, size_t len)</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+WriteData
+452</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+Finalize
+597</t>
+  </si>
+  <si>
+    <r>
+      <t>memcpy(tmptrc, m_bufClearDataForAES, cbReadyToAesCipher</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>];</t>
+    </r>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+Finalize
+598</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+Finalize
+604</t>
+  </si>
+  <si>
+    <t>tmptrc should be checked for NULL</t>
+  </si>
+  <si>
+    <t>char* tmptrc = new char[cbReadyToAesCipher];
+            memcpy(tmptrc, m_bufClearDataForAES, cbReadyToAesCipher];</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+Finalize
+596</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+Finalize
+649</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+Finalize
+664</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+Finalize
+666</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+TMP_CodeCredit_CheckPANInsideBINs
+51</t>
+  </si>
+  <si>
+    <t>IsoBuf should be NULL checked</t>
+  </si>
+  <si>
+    <t>Risk</t>
+  </si>
+  <si>
+    <t>If buffers are not explicitly NULL terminated, may lead to memory access violation when used with string library functions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passing buffer and index both as a function parameters is in a scenario like this is bad coding practice and makes the function vulnarable. Caller function logic should be corrected and pointer should be passed. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Always check NULL before de-referenced,  a thumb rule, no matter how many extra instructions it might add up to, we are have no such memory contraints. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">strlen( PanValue )
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>OK But..</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Calculate string length once and use everywhere unless the PanValue is altered
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Reccomended</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+We have run the loop and have the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>unIndexPan</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> as PAN leangth. Just use this!! </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>OK But..</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+memset( INC_Bin, '0', NC_MD_239 );
+    memcpy( INC_Bin, PanValue, strlen( PanValue ) );
+    INC_Bin[NC_MD_239] = 0;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Reccomended</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+memset( INC_Bin, '0', NC_MD_239 );
+    memcpy( INC_Bin, PanValue, unIndexPan );
+    INC_Bin[unIndexPan] = 0;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Do the same SUC_Bin buffer.</t>
+    </r>
+  </si>
+  <si>
+    <t>Use of memcmp/strncmp reccomended</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+TMP_CodeCredit_CheckServiceCode
+121</t>
+  </si>
+  <si>
+    <t>INF_CodeService [NC_MD_287] = 0;
+SUF_CodeService [NC_MD_287] = 0;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">INF_CodeService [NC_MD_287] = 0;
+SUF_CodeService [NC_MD_287] = 0;
+Buffer OVERFLOW
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Define</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+char INF_CodeService[NC_MD_287</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> + 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>];
+char SUF_CodeService[NC_MD_287</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> + 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>];</t>
+    </r>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+TMP_CodeCredit_CheckServiceCode
+109</t>
+  </si>
+  <si>
+    <t>CodeReview1.cpp
+TMP_CodeCredit_CheckServiceCode
+128</t>
+  </si>
+  <si>
+    <t>ServiceCode=strtoul((char *)pucCardServiceCode,NULL,0);</t>
+  </si>
+  <si>
+    <t>pucCardServiceCode should be NULL checked
+pucCardServiceCode should be NULL checked
+ideally, all pointer parameters must be NULL checked at the beginning of the function.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">LOOPING:
+for loop is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>OK</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+BUT…
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>If condition with 3 checks would suffice for service code</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>for(unIndexCodeService = 0; unIndexCodeService &lt; NC_MD_287 ; unIndexCodeService++)
+ {
+  if(SUF_CodeService[unIndexCodeService] == '*') 
+  {
+   SUF_wildcard=1;
+  } 
+  if (INF_CodeService[unIndexCodeService] == '*')
+  {
+   INF_wildcard=1;
+  }
+ }</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">if unTailleMax &gt; NC_MD_239 will lead to buffer overflow
 strncpy( acInfPlage,(const char*) &amp;pCurrentEnreg[unFileBeginningIndex], unTailleMax );
@@ -395,7 +855,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color indexed="8"/>
+        <color rgb="FF00B050"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
@@ -409,251 +869,59 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">
-strncpy( acInfPlage,(const char*) &amp;pCurrentEnreg[unFileBeginningIndex], sizeof( acInfPlage ));</t>
+strncpy( acInfPlage,(const char*) &amp;pCurrentEnreg[unFileBeginningIndex], sizeof( acInfPlage ) - 1);
+Ensure buffer has space holder for NULL
+char acInfPlage[NC_MD_239</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">
-szHexIV[32] = 0; is a OVERFLOW
-Buffer size should be 32 + 1
-char szHexIV[32 + 1] = {0};</t>
-  </si>
-  <si>
-    <t>un-compiled code? :-)
-Really unexpected !!!</t>
-  </si>
-  <si>
-    <t>Heap overflow
-tmptrc[cbReadyToAesCipher] = 0;</t>
-  </si>
-  <si>
-    <t>error</t>
-  </si>
-  <si>
-    <t>CodeReview1.cpp</t>
-  </si>
-  <si>
-    <t>Invalid number of character &amp;amp;#039;[&amp;amp;#039; when no macros are defined." verbose="Invalid number of character &amp;amp;#039;[&amp;amp;#039; when no macros are defined.</t>
-  </si>
-  <si>
-    <t>Invalid number of character &amp;amp;#039;[&amp;amp;#039; when these macros are defined: &amp;amp;#039;LOG_ALL&amp;amp;#039;." verbose="Invalid number of character &amp;amp;#039;[&amp;amp;#039; when these macros are defined: &amp;amp;#039;LOG_ALL&amp;amp;#039;.</t>
-  </si>
-  <si>
-    <t>CodeReview1.cpp
-WriteData</t>
-  </si>
-  <si>
-    <t>CodeReview1.cpp
-TMP_CodeCredit_CheckPANInsideBINs
-38</t>
-  </si>
-  <si>
-    <t>Passing buffer Index(es) as part function parameters is NOT reccomended. Address passing should be handled by the caller function.
-Also, use sizeof() for length to ensure fewer modifications in case where we change the buffer size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INCORRECT LENGTH passed.
-sizeof(IsoBuf) gives length of pointer.
-Use sizeof(PanValue) - 1 with strncpy function if IsoBuf is expected to be NULL terminated
-If NOT Caller must pass the length
-</t>
-  </si>
-  <si>
-    <t>CodeReview1.cpp
-TMP_CodeCredit_CheckPANInsideBINs
-52</t>
-  </si>
-  <si>
-    <t>CodeReview1.cpp
-TMP_CodeCredit_CheckPANInsideBINs
-58</t>
-  </si>
-  <si>
-    <t>CodeReview1.cpp
-TMP_CodeCredit_CheckPANInsideBINs
-65</t>
-  </si>
-  <si>
-    <t>CodeReview1.cpp
-TMP_CodeCredit_CheckPANInsideBINs
-70, 77</t>
-  </si>
-  <si>
-    <t>CodeReview1.cpp
-TMP_CodeCredit_CheckPANInsideBINs
-70</t>
-  </si>
-  <si>
-    <t>CodeReview1.cpp
-TMP_CodeCredit_CheckPANInsideBINs
-82</t>
-  </si>
-  <si>
-    <t>CodeReview1.cpp
-TMP_CodeCredit_CheckPANInsideBINs
-109</t>
-  </si>
-  <si>
-    <t>CodeReview1.cpp
-TMP_CodeCredit_CheckPANInsideBINs
-121</t>
-  </si>
-  <si>
-    <t>CodeReview1.cpp
-TMP_CodeCredit_CheckServiceCode
-130</t>
-  </si>
-  <si>
-    <t>CodeReview1.cpp
-TMP_CodeCredit_CheckServiceCode
-159</t>
-  </si>
-  <si>
-    <t>CodeReview1.cpp
-TMP_CodeCredit_CheckServiceCode
-238</t>
-  </si>
-  <si>
-    <t>CodeReview1.cpp
-TMP_CodeCredit_GetSameNumber
-257</t>
-  </si>
-  <si>
-    <t>acInfPlage NOT initialized</t>
-  </si>
-  <si>
-    <t>char acInfPlage[NC_MD_239]; //NC_MD_239 est la plus grande taille Ã  regarder</t>
-  </si>
-  <si>
-    <t>CodeReview1.cpp
-TMP_CodeCredit_GetSameNumber
-261</t>
-  </si>
-  <si>
-    <t>CodeReview1.cpp
-TMP_CodeCredit_GetSameNumber
-264</t>
-  </si>
-  <si>
-    <t>strncpy( acInfPlage,(const char*) &amp;pCurrentEnreg[unFileBeginningIndex], unTailleMax );</t>
-  </si>
-  <si>
-    <t>CodeReview1.cpp
-TMP_CodeCredit_GetSameNumber
-267</t>
-  </si>
-  <si>
-    <t>CodeReview1.cpp
-Init
-345</t>
-  </si>
-  <si>
-    <t>CodeReview1.cpp
-Init
-370</t>
-  </si>
-  <si>
-    <t>CodeReview1.cpp
-Init
-363</t>
-  </si>
-  <si>
-    <t>FileUtils::GetTempFilePath (pszOutputFilePath, true, "VF_", m_szTmpOutputFilePath, MAX_PATH);</t>
-  </si>
-  <si>
-    <t>Use sizeof() for length</t>
-  </si>
-  <si>
-    <t>CodeReview1.cpp
-Init
-339</t>
-  </si>
-  <si>
-    <t>CodeReview1.cpp
-Init
-423</t>
-  </si>
-  <si>
-    <t>CodeReview1.cpp
-WriteData
-507</t>
-  </si>
-  <si>
-    <t>data should be checked for NULL</t>
-  </si>
-  <si>
-    <t>bool SecuredFileWriter::WriteData (const char *data, size_t len)</t>
-  </si>
-  <si>
-    <t>CodeReview1.cpp
-WriteData
-452</t>
-  </si>
-  <si>
-    <t>This function is heavily depending on Class variables cannot say whether it is OK or not, as do not know the context</t>
-  </si>
-  <si>
-    <t>CodeReview1.cpp
-Finalize
-597</t>
-  </si>
-  <si>
     <r>
-      <t>memcpy(tmptrc, m_bufClearDataForAES, cbReadyToAesCipher</t>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> + 1</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
+        <color indexed="8"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>];</t>
+      <t xml:space="preserve">]; </t>
     </r>
   </si>
   <si>
+    <t>BUFFER OVERFLOW if unTailleMax &gt; NC_MD_239
+re-write this function</t>
+  </si>
+  <si>
+    <t>bool SecuredFileWriter::Init (const char *pszOutputFilePath, const char *pszPublicKeyFilePath, bool fOutputBase64Only)</t>
+  </si>
+  <si>
+    <t>Use sizeof() to pass the length
+strncpy (m_szOutputFilePath, pszOutputFilePath, sizeof((m_szOutputFilePath));</t>
+  </si>
+  <si>
+    <t>*m_szTmpOutputFilePath = 0;
+USE m_szTmpOutputFilePath[0] = 0; for clarity</t>
+  </si>
+  <si>
+    <t>*m_szTmpOutputFilePath = 0;</t>
+  </si>
+  <si>
     <t>CodeReview1.cpp
-Finalize
-598</t>
-  </si>
-  <si>
-    <t>CodeReview1.cpp
-Finalize
-604</t>
-  </si>
-  <si>
-    <t>tmptrc should be checked for NULL</t>
-  </si>
-  <si>
-    <t>char* tmptrc = new char[cbReadyToAesCipher];
-            memcpy(tmptrc, m_bufClearDataForAES, cbReadyToAesCipher];</t>
-  </si>
-  <si>
-    <t>CodeReview1.cpp
-Finalize
-596</t>
-  </si>
-  <si>
-    <t>CodeReview1.cpp
-Finalize
-649</t>
-  </si>
-  <si>
-    <t>CodeReview1.cpp
-Finalize
-664</t>
-  </si>
-  <si>
-    <t>CodeReview1.cpp
-Finalize
-666</t>
+Init
+394, 408</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -682,25 +950,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF00B050"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
@@ -713,8 +962,33 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -742,6 +1016,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -872,7 +1152,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -892,9 +1172,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -954,84 +1231,27 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel_BuiltIn_Heading 1" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="77">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="69">
     <dxf>
       <font>
         <b val="0"/>
@@ -2081,7 +2301,7 @@
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.33203125" customWidth="1"/>
-    <col min="2" max="2" width="27.33203125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" style="16" customWidth="1"/>
     <col min="3" max="3" width="42.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.5546875" customWidth="1"/>
@@ -2111,11 +2331,11 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="18">
+      <c r="A2" s="17">
         <v>43091</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>69</v>
+      <c r="B2" s="15" t="s">
+        <v>63</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5" t="s">
@@ -2131,7 +2351,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
-      <c r="B3" s="16"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -2141,7 +2361,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
-      <c r="B4" s="16"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -2154,7 +2374,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
-      <c r="B5" s="16"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -2167,7 +2387,7 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
-      <c r="B6" s="16"/>
+      <c r="B6" s="15"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -2177,7 +2397,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
-      <c r="B7" s="16"/>
+      <c r="B7" s="15"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -2187,7 +2407,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
-      <c r="B8" s="16"/>
+      <c r="B8" s="15"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
@@ -2197,7 +2417,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
-      <c r="B9" s="16"/>
+      <c r="B9" s="15"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
@@ -2207,7 +2427,7 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
-      <c r="B10" s="16"/>
+      <c r="B10" s="15"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -2217,7 +2437,7 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
-      <c r="B11" s="16"/>
+      <c r="B11" s="15"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -2227,7 +2447,7 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
-      <c r="B12" s="16"/>
+      <c r="B12" s="15"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -2237,7 +2457,7 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
-      <c r="B13" s="16"/>
+      <c r="B13" s="15"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
@@ -2247,147 +2467,147 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
-      <c r="B14" s="16"/>
+      <c r="B14" s="15"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
-      <c r="B15" s="16"/>
+      <c r="B15" s="15"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
-      <c r="B16" s="16"/>
+      <c r="B16" s="15"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
-      <c r="B17" s="16"/>
+      <c r="B17" s="15"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
-      <c r="B18" s="16"/>
+      <c r="B18" s="15"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
-      <c r="B19" s="16"/>
+      <c r="B19" s="15"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
-      <c r="B20" s="16"/>
+      <c r="B20" s="15"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
-      <c r="B21" s="16"/>
+      <c r="B21" s="15"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
-      <c r="B22" s="16"/>
+      <c r="B22" s="15"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
-      <c r="B23" s="16"/>
+      <c r="B23" s="15"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
-      <c r="B24" s="16"/>
+      <c r="B24" s="15"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
-      <c r="B25" s="16"/>
+      <c r="B25" s="15"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
-      <c r="B26" s="16"/>
+      <c r="B26" s="15"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
-      <c r="B27" s="16"/>
+      <c r="B27" s="15"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
-      <c r="B28" s="16"/>
+      <c r="B28" s="15"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
-      <c r="B29" s="16"/>
+      <c r="B29" s="15"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
-      <c r="B30" s="16"/>
+      <c r="B30" s="15"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
-      <c r="B31" s="16"/>
+      <c r="B31" s="15"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
-      <c r="B32" s="16"/>
+      <c r="B32" s="15"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
-      <c r="B33" s="16"/>
+      <c r="B33" s="15"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
-      <c r="B34" s="16"/>
+      <c r="B34" s="15"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
@@ -2426,18 +2646,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:D34">
-    <cfRule type="cellIs" dxfId="76" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="3" stopIfTrue="1" operator="equal">
       <formula>$Q$2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="4" stopIfTrue="1" operator="equal">
       <formula>$Q$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E34">
-    <cfRule type="cellIs" dxfId="74" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="1" stopIfTrue="1" operator="equal">
       <formula>$Q$2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="2" stopIfTrue="1" operator="equal">
       <formula>$Q$1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2453,20 +2673,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="46" customWidth="1"/>
-    <col min="2" max="2" width="40.88671875" style="15" customWidth="1"/>
-    <col min="3" max="3" width="61.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="80.77734375" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.44140625" customWidth="1"/>
-    <col min="6" max="6" width="19.88671875" style="13" customWidth="1"/>
+    <col min="2" max="2" width="36.33203125" style="14" customWidth="1"/>
+    <col min="3" max="3" width="56.44140625" customWidth="1"/>
+    <col min="4" max="4" width="76.21875" style="35" customWidth="1"/>
+    <col min="5" max="5" width="22.44140625" style="36" customWidth="1"/>
+    <col min="6" max="6" width="19.88671875" style="39" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2479,602 +2699,680 @@
       <c r="C1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="32" t="s">
         <v>24</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="9"/>
+      <c r="F1" s="1" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="2" spans="1:6" ht="227.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="40" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="227.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="37" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="227.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="37" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="227.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="37"/>
+    </row>
+    <row r="6" spans="1:6" ht="81.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="38"/>
+    </row>
+    <row r="7" spans="1:6" ht="86.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="172.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="D8" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="37"/>
+    </row>
+    <row r="9" spans="1:6" ht="227.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D9" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="37"/>
+    </row>
+    <row r="10" spans="1:6" ht="134.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="37"/>
+    </row>
+    <row r="11" spans="1:6" ht="134.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="37"/>
+    </row>
+    <row r="12" spans="1:6" ht="134.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="33"/>
+      <c r="E12" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="37"/>
+    </row>
+    <row r="13" spans="1:6" ht="134.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="37"/>
+    </row>
+    <row r="14" spans="1:6" ht="134.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="D14" s="33" t="s">
+        <v>131</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="37"/>
+    </row>
+    <row r="15" spans="1:6" ht="134.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="37"/>
+    </row>
+    <row r="16" spans="1:6" ht="134.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="D16" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="37"/>
+    </row>
+    <row r="17" spans="1:6" ht="134.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="37"/>
+    </row>
+    <row r="18" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="34"/>
+      <c r="E18" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" s="37"/>
+    </row>
+    <row r="20" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="144" x14ac:dyDescent="0.3">
+      <c r="A22" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="D22" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="144" x14ac:dyDescent="0.3">
+      <c r="A23" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="D23" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="35" t="s">
+        <v>137</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="D25" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A27" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="D27" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A28" s="31" t="s">
+        <v>141</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="D28" s="35" t="s">
+        <v>140</v>
+      </c>
+      <c r="E28" s="9"/>
+    </row>
+    <row r="29" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A29" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="D29" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" t="s">
+        <v>104</v>
+      </c>
+      <c r="D30" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A31" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A32" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" t="s">
+        <v>55</v>
+      </c>
+      <c r="D32" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A33" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="D33" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A34" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="15" t="s">
+      <c r="D34" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A35" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" t="s">
+        <v>111</v>
+      </c>
+      <c r="D35" s="35" t="s">
+        <v>112</v>
+      </c>
+      <c r="E35" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="10"/>
-    </row>
-    <row r="3" spans="1:6" ht="227.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="D3" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="15" t="s">
+    </row>
+    <row r="36" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A36" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="D36" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="E36" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="10"/>
-    </row>
-    <row r="4" spans="1:6" ht="227.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="D4" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="10"/>
-    </row>
-    <row r="5" spans="1:6" ht="81.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="B5" s="15" t="s">
+    </row>
+    <row r="37" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A37" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="B37" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D5" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="E5" s="15" t="s">
+      <c r="C37" t="s">
+        <v>58</v>
+      </c>
+      <c r="D37" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="E37" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="11"/>
-    </row>
-    <row r="6" spans="1:6" ht="86.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="B6" s="15" t="s">
+    </row>
+    <row r="38" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A38" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="B38" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="15" t="s">
+      <c r="C38" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="D38" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="E38" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="12"/>
-    </row>
-    <row r="7" spans="1:6" ht="111.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="B7" s="15" t="s">
+    </row>
+    <row r="39" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A39" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="B39" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="10"/>
-    </row>
-    <row r="8" spans="1:6" ht="227.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="10"/>
-    </row>
-    <row r="9" spans="1:6" ht="134.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="10"/>
-    </row>
-    <row r="10" spans="1:6" ht="134.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="10"/>
-    </row>
-    <row r="11" spans="1:6" ht="134.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="34"/>
-      <c r="E11" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="10"/>
-    </row>
-    <row r="12" spans="1:6" ht="134.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D12" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="10"/>
-    </row>
-    <row r="13" spans="1:6" ht="134.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="D13" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" s="10"/>
-    </row>
-    <row r="14" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" s="35"/>
-      <c r="E14" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="32" t="s">
-        <v>98</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="D15" s="36" t="s">
-        <v>100</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="10"/>
-    </row>
-    <row r="16" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="36" t="s">
-        <v>48</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="32" t="s">
-        <v>102</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="D17" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="D18" s="36" t="s">
-        <v>103</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="32" t="s">
-        <v>104</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="32" t="s">
-        <v>105</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="32" t="s">
-        <v>107</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="D21" s="36" t="s">
-        <v>55</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="32" t="s">
-        <v>106</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="32" t="s">
-        <v>109</v>
-      </c>
-      <c r="D22" s="36" t="s">
-        <v>108</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="32" t="s">
-        <v>110</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="D23" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A24" s="32" t="s">
-        <v>111</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="32" t="s">
-        <v>76</v>
-      </c>
-      <c r="D24" s="36" t="s">
-        <v>58</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A26" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="D26" s="36" t="s">
-        <v>59</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A27" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" t="s">
-        <v>113</v>
-      </c>
-      <c r="D27" s="36" t="s">
-        <v>114</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C28" s="32" t="s">
-        <v>116</v>
-      </c>
-      <c r="E28" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A29" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="C39" t="s">
         <v>61</v>
       </c>
-      <c r="D29" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="E29" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A30" s="32" t="s">
-        <v>117</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="D30" s="36" t="s">
-        <v>118</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A31" s="32" t="s">
-        <v>119</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C31" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="D31" s="36" t="s">
+      <c r="D39" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="E31" s="15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A32" s="32" t="s">
-        <v>120</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C32" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="D32" s="36" t="s">
-        <v>59</v>
-      </c>
-      <c r="E32" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A33" s="32" t="s">
-        <v>123</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C33" t="s">
-        <v>121</v>
-      </c>
-      <c r="D33" s="36" t="s">
-        <v>122</v>
-      </c>
-      <c r="E33" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A34" s="32" t="s">
-        <v>124</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C34" t="s">
-        <v>64</v>
-      </c>
-      <c r="D34" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="E34" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A35" s="32" t="s">
-        <v>125</v>
-      </c>
-      <c r="B35" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C35" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="D35" s="36" t="s">
-        <v>66</v>
-      </c>
-      <c r="E35" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A36" s="32" t="s">
-        <v>126</v>
-      </c>
-      <c r="B36" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C36" t="s">
-        <v>67</v>
-      </c>
-      <c r="D36" s="36" t="s">
-        <v>68</v>
-      </c>
-      <c r="E36" s="15" t="s">
+      <c r="E39" s="9" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B26:B36 B2:B24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B36 B37:B39">
       <formula1>Rules</formula1>
     </dataValidation>
   </dataValidations>
@@ -3108,7 +3406,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E5:E7 E9 E25 E37:E58</xm:sqref>
+          <xm:sqref>E6:E8 E10 E40:E61</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="63" stopIfTrue="1" operator="equal" id="{602A14BB-9BDF-4C1A-812D-6A0EB6747D9F}">
@@ -3135,7 +3433,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E3</xm:sqref>
+          <xm:sqref>E3:E4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="61" stopIfTrue="1" operator="equal" id="{8C5A4143-3864-49CB-86A9-B0F33F284F6A}">
@@ -3189,7 +3487,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E4</xm:sqref>
+          <xm:sqref>E5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="57" stopIfTrue="1" operator="equal" id="{94A6B6BB-4DDE-4209-B1AA-4070E24FA1BF}">
@@ -3216,7 +3514,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E8</xm:sqref>
+          <xm:sqref>E9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="55" stopIfTrue="1" operator="equal" id="{E9316EA5-6F05-40B4-A750-5EEF9C6F8A31}">
@@ -3243,7 +3541,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E10</xm:sqref>
+          <xm:sqref>E11</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="53" stopIfTrue="1" operator="equal" id="{85C59230-A024-4095-B166-305386F38BD8}">
@@ -3270,7 +3568,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E11</xm:sqref>
+          <xm:sqref>E12:E14</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="51" stopIfTrue="1" operator="equal" id="{C1A10AEC-D27E-497B-86D5-140AEFADD175}">
@@ -3297,7 +3595,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E12</xm:sqref>
+          <xm:sqref>E15:E16</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="49" stopIfTrue="1" operator="equal" id="{A4551ED4-8FB8-4495-830B-4AFDD0CBC3D5}">
@@ -3324,7 +3622,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E13</xm:sqref>
+          <xm:sqref>E17</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="47" stopIfTrue="1" operator="equal" id="{AB48A264-90BF-4883-9FA6-004AB47A8687}">
@@ -3351,7 +3649,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E14</xm:sqref>
+          <xm:sqref>E18</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="45" stopIfTrue="1" operator="equal" id="{6CF7CF66-F40A-4BF2-989A-F0A9EA1207C0}">
@@ -3378,7 +3676,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E16</xm:sqref>
+          <xm:sqref>E20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="43" stopIfTrue="1" operator="equal" id="{723D429E-2271-49E4-BABA-ED32592ADEA1}">
@@ -3405,7 +3703,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E17</xm:sqref>
+          <xm:sqref>E21</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="41" stopIfTrue="1" operator="equal" id="{0A5A250E-298D-45D2-B4F7-1AA08E820D92}">
@@ -3432,7 +3730,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E18</xm:sqref>
+          <xm:sqref>E22</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="39" stopIfTrue="1" operator="equal" id="{509068B4-3D5A-4625-A659-7B7771383D1D}">
@@ -3459,7 +3757,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E19</xm:sqref>
+          <xm:sqref>E23:E24</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="37" stopIfTrue="1" operator="equal" id="{1806BF15-7656-4D02-891F-C2C88F533618}">
@@ -3486,7 +3784,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E20</xm:sqref>
+          <xm:sqref>E25</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="35" stopIfTrue="1" operator="equal" id="{603A0457-A83C-4696-81AE-C6601F79E859}">
@@ -3513,10 +3811,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E21</xm:sqref>
+          <xm:sqref>E26</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="33" stopIfTrue="1" operator="equal" id="{42E9A256-6C7C-4981-B010-4099E20FABCA}">
+          <x14:cfRule type="cellIs" priority="29" stopIfTrue="1" operator="equal" id="{57CC6C1A-4D4E-49B6-832C-89A45E88CFE7}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -3526,7 +3824,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="34" stopIfTrue="1" operator="equal" id="{2CB1E213-6AEA-4B1A-AB01-53AAD0D5790F}">
+          <x14:cfRule type="cellIs" priority="30" stopIfTrue="1" operator="equal" id="{315E6B91-235A-445B-B517-F9C5B1D37EAE}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -3540,10 +3838,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E23</xm:sqref>
+          <xm:sqref>E29</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="29" stopIfTrue="1" operator="equal" id="{57CC6C1A-4D4E-49B6-832C-89A45E88CFE7}">
+          <x14:cfRule type="cellIs" priority="27" stopIfTrue="1" operator="equal" id="{4B1E35FF-0116-4119-9C46-B62114BCB4D1}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -3553,7 +3851,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="30" stopIfTrue="1" operator="equal" id="{315E6B91-235A-445B-B517-F9C5B1D37EAE}">
+          <x14:cfRule type="cellIs" priority="28" stopIfTrue="1" operator="equal" id="{1BEF4AE7-FF76-48FD-815B-DF262AE3CFE0}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -3567,10 +3865,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E24</xm:sqref>
+          <xm:sqref>E31</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="27" stopIfTrue="1" operator="equal" id="{4B1E35FF-0116-4119-9C46-B62114BCB4D1}">
+          <x14:cfRule type="cellIs" priority="25" stopIfTrue="1" operator="equal" id="{56A818B0-64D8-4601-90CC-C6EDD507EA9C}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -3580,7 +3878,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="28" stopIfTrue="1" operator="equal" id="{1BEF4AE7-FF76-48FD-815B-DF262AE3CFE0}">
+          <x14:cfRule type="cellIs" priority="26" stopIfTrue="1" operator="equal" id="{17B3CA77-595F-408E-BE76-D589997E775B}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -3594,10 +3892,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E26</xm:sqref>
+          <xm:sqref>E30</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="25" stopIfTrue="1" operator="equal" id="{56A818B0-64D8-4601-90CC-C6EDD507EA9C}">
+          <x14:cfRule type="cellIs" priority="21" stopIfTrue="1" operator="equal" id="{51379761-3831-4490-968E-247ABD1A188C}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -3607,7 +3905,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="26" stopIfTrue="1" operator="equal" id="{17B3CA77-595F-408E-BE76-D589997E775B}">
+          <x14:cfRule type="cellIs" priority="22" stopIfTrue="1" operator="equal" id="{71DA6DDA-5280-4ADC-A4F0-C4A726FF5E8A}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -3621,10 +3919,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E27</xm:sqref>
+          <xm:sqref>E32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="23" stopIfTrue="1" operator="equal" id="{8EFB9414-826C-4022-A42F-DBF2E2ACBD12}">
+          <x14:cfRule type="cellIs" priority="19" stopIfTrue="1" operator="equal" id="{7000E78B-8344-4F21-8566-805BB092F3D8}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -3634,7 +3932,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="24" stopIfTrue="1" operator="equal" id="{37CA990F-0EB9-4F54-968D-AF772C0F3C2F}">
+          <x14:cfRule type="cellIs" priority="20" stopIfTrue="1" operator="equal" id="{3F33EA94-08A9-4DCF-BEC6-E70B2D7DC02D}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -3648,10 +3946,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E28</xm:sqref>
+          <xm:sqref>E33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="21" stopIfTrue="1" operator="equal" id="{51379761-3831-4490-968E-247ABD1A188C}">
+          <x14:cfRule type="cellIs" priority="17" stopIfTrue="1" operator="equal" id="{9A282710-C433-496A-A098-FAD9D4C6A268}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -3661,7 +3959,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="22" stopIfTrue="1" operator="equal" id="{71DA6DDA-5280-4ADC-A4F0-C4A726FF5E8A}">
+          <x14:cfRule type="cellIs" priority="18" stopIfTrue="1" operator="equal" id="{D6811E4F-319E-4C10-8B82-9D4173AF56A0}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -3675,10 +3973,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E29</xm:sqref>
+          <xm:sqref>E34</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="19" stopIfTrue="1" operator="equal" id="{7000E78B-8344-4F21-8566-805BB092F3D8}">
+          <x14:cfRule type="cellIs" priority="15" stopIfTrue="1" operator="equal" id="{56B58C0B-73C7-45C7-880B-A8A864AEEB5F}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -3688,7 +3986,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="20" stopIfTrue="1" operator="equal" id="{3F33EA94-08A9-4DCF-BEC6-E70B2D7DC02D}">
+          <x14:cfRule type="cellIs" priority="16" stopIfTrue="1" operator="equal" id="{7F7F6FA1-0D19-4448-8002-D9882A8ABA6C}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -3702,10 +4000,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E30</xm:sqref>
+          <xm:sqref>E36</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="17" stopIfTrue="1" operator="equal" id="{9A282710-C433-496A-A098-FAD9D4C6A268}">
+          <x14:cfRule type="cellIs" priority="13" stopIfTrue="1" operator="equal" id="{F8759862-0F30-4D84-AAFA-113B17483CFF}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -3715,7 +4013,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="18" stopIfTrue="1" operator="equal" id="{D6811E4F-319E-4C10-8B82-9D4173AF56A0}">
+          <x14:cfRule type="cellIs" priority="14" stopIfTrue="1" operator="equal" id="{E858A037-4BA5-410C-B670-8D7A8C222E96}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -3729,10 +4027,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E31</xm:sqref>
+          <xm:sqref>E35</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="15" stopIfTrue="1" operator="equal" id="{56B58C0B-73C7-45C7-880B-A8A864AEEB5F}">
+          <x14:cfRule type="cellIs" priority="11" stopIfTrue="1" operator="equal" id="{74263FAC-CF77-4538-BBD8-73F2C08179CC}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -3742,7 +4040,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="16" stopIfTrue="1" operator="equal" id="{7F7F6FA1-0D19-4448-8002-D9882A8ABA6C}">
+          <x14:cfRule type="cellIs" priority="12" stopIfTrue="1" operator="equal" id="{A3DD3372-D965-4C24-85A4-EA6E4382C7D6}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -3756,10 +4054,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E32</xm:sqref>
+          <xm:sqref>E37</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="13" stopIfTrue="1" operator="equal" id="{F8759862-0F30-4D84-AAFA-113B17483CFF}">
+          <x14:cfRule type="cellIs" priority="9" stopIfTrue="1" operator="equal" id="{BC224CCD-AED0-47E8-A807-BC68B81EBB46}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -3769,7 +4067,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="14" stopIfTrue="1" operator="equal" id="{E858A037-4BA5-410C-B670-8D7A8C222E96}">
+          <x14:cfRule type="cellIs" priority="10" stopIfTrue="1" operator="equal" id="{13CDBA54-459C-429C-976B-B6B80CF25615}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -3783,10 +4081,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E33</xm:sqref>
+          <xm:sqref>E38</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="11" stopIfTrue="1" operator="equal" id="{74263FAC-CF77-4538-BBD8-73F2C08179CC}">
+          <x14:cfRule type="cellIs" priority="7" stopIfTrue="1" operator="equal" id="{FA246ABD-99D2-48A5-B712-63D5DE1373BB}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -3796,7 +4094,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="12" stopIfTrue="1" operator="equal" id="{A3DD3372-D965-4C24-85A4-EA6E4382C7D6}">
+          <x14:cfRule type="cellIs" priority="8" stopIfTrue="1" operator="equal" id="{ACD219FD-8B2C-4CEC-B767-5D010594E27A}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -3810,10 +4108,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E34</xm:sqref>
+          <xm:sqref>E39</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="9" stopIfTrue="1" operator="equal" id="{BC224CCD-AED0-47E8-A807-BC68B81EBB46}">
+          <x14:cfRule type="cellIs" priority="3" stopIfTrue="1" operator="equal" id="{527FF2D0-730F-4E2D-BB75-072DDE5D9BC0}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -3823,7 +4121,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="10" stopIfTrue="1" operator="equal" id="{13CDBA54-459C-429C-976B-B6B80CF25615}">
+          <x14:cfRule type="cellIs" priority="4" stopIfTrue="1" operator="equal" id="{A6CFC000-223C-4E5D-9B15-371B831ADF9F}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -3837,10 +4135,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E35</xm:sqref>
+          <xm:sqref>E27:E28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="7" stopIfTrue="1" operator="equal" id="{FA246ABD-99D2-48A5-B712-63D5DE1373BB}">
+          <x14:cfRule type="cellIs" priority="1" stopIfTrue="1" operator="equal" id="{77049A23-0BD6-4761-A28E-A3AA974475F7}">
             <xm:f>History!$Q$5</xm:f>
             <x14:dxf>
               <fill>
@@ -3850,7 +4148,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="8" stopIfTrue="1" operator="equal" id="{ACD219FD-8B2C-4CEC-B767-5D010594E27A}">
+          <x14:cfRule type="cellIs" priority="2" stopIfTrue="1" operator="equal" id="{4462B2BB-D1CC-4F36-B92C-4D660C855A60}">
             <xm:f>History!$Q$4</xm:f>
             <x14:dxf>
               <font>
@@ -3864,61 +4162,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E36</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="3" stopIfTrue="1" operator="equal" id="{527FF2D0-730F-4E2D-BB75-072DDE5D9BC0}">
-            <xm:f>History!$Q$5</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFFC000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="4" stopIfTrue="1" operator="equal" id="{A6CFC000-223C-4E5D-9B15-371B831ADF9F}">
-            <xm:f>History!$Q$4</xm:f>
-            <x14:dxf>
-              <font>
-                <b/>
-                <i val="0"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFF0000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>E22</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="1" stopIfTrue="1" operator="equal" id="{77049A23-0BD6-4761-A28E-A3AA974475F7}">
-            <xm:f>History!$Q$5</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFFC000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="2" stopIfTrue="1" operator="equal" id="{4462B2BB-D1CC-4F36-B92C-4D660C855A60}">
-            <xm:f>History!$Q$4</xm:f>
-            <x14:dxf>
-              <font>
-                <b/>
-                <i val="0"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFF0000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>E15</xm:sqref>
+          <xm:sqref>E19</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -3928,7 +4172,7 @@
           <x14:formula1>
             <xm:f>History!$Q$4:$Q$5</xm:f>
           </x14:formula1>
-          <xm:sqref>E26:E36 E2:E24</xm:sqref>
+          <xm:sqref>E2:E36 E37:E39</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3967,385 +4211,385 @@
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="B2" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="C2" s="20">
+    <row r="2" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="19">
         <v>597</v>
       </c>
-      <c r="D2" s="21" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="B3" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="C3" s="20">
+      <c r="D2" s="20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="19">
         <v>597</v>
       </c>
-      <c r="D3" s="24" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="22"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="24"/>
-    </row>
-    <row r="5" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="22"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="21"/>
-    </row>
-    <row r="6" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="22"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="25"/>
-    </row>
-    <row r="7" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="22"/>
-      <c r="B7" s="30"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="25"/>
-    </row>
-    <row r="8" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="22"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="24"/>
-    </row>
-    <row r="9" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="22"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="24"/>
-    </row>
-    <row r="10" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="22"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="24"/>
-    </row>
-    <row r="11" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="22"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="24"/>
-    </row>
-    <row r="12" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="22"/>
-      <c r="B12" s="30"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="24"/>
-    </row>
-    <row r="13" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="22"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="25"/>
-    </row>
-    <row r="14" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="22"/>
-      <c r="B14" s="30"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="25"/>
-    </row>
-    <row r="15" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="22"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="25"/>
-    </row>
-    <row r="16" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="22"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="25"/>
-    </row>
-    <row r="17" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="22"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="25"/>
-    </row>
-    <row r="18" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="22"/>
-      <c r="B18" s="30"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="25"/>
-    </row>
-    <row r="19" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="22"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="25"/>
-    </row>
-    <row r="20" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="22"/>
-      <c r="B20" s="30"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="25"/>
-    </row>
-    <row r="21" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="22"/>
-      <c r="B21" s="30"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="25"/>
-    </row>
-    <row r="22" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="22"/>
-      <c r="B22" s="30"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="25"/>
-    </row>
-    <row r="23" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="22"/>
-      <c r="B23" s="30"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="25"/>
-    </row>
-    <row r="24" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="22"/>
-      <c r="B24" s="30"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="25"/>
-    </row>
-    <row r="25" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="22"/>
-      <c r="B25" s="30"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="25"/>
-    </row>
-    <row r="26" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="22"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="25"/>
-    </row>
-    <row r="27" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="22"/>
-      <c r="B27" s="30"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="25"/>
-    </row>
-    <row r="28" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="22"/>
-      <c r="B28" s="30"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="25"/>
-    </row>
-    <row r="29" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="22"/>
-      <c r="B29" s="30"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="25"/>
-    </row>
-    <row r="30" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="22"/>
-      <c r="B30" s="30"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="25"/>
-    </row>
-    <row r="31" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="22"/>
-      <c r="B31" s="30"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="25"/>
-    </row>
-    <row r="32" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="22"/>
-      <c r="B32" s="30"/>
-      <c r="C32" s="23"/>
-      <c r="D32" s="25"/>
-    </row>
-    <row r="33" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="22"/>
-      <c r="B33" s="30"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="25"/>
-    </row>
-    <row r="34" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="22"/>
-      <c r="B34" s="30"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="25"/>
-    </row>
-    <row r="35" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="22"/>
-      <c r="B35" s="30"/>
-      <c r="C35" s="23"/>
-      <c r="D35" s="25"/>
-    </row>
-    <row r="36" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="22"/>
-      <c r="B36" s="30"/>
-      <c r="C36" s="23"/>
-      <c r="D36" s="24"/>
-    </row>
-    <row r="37" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="22"/>
-      <c r="B37" s="30"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="25"/>
-    </row>
-    <row r="38" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="22"/>
-      <c r="B38" s="30"/>
-      <c r="C38" s="23"/>
-      <c r="D38" s="25"/>
-    </row>
-    <row r="39" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="22"/>
-      <c r="B39" s="30"/>
-      <c r="C39" s="23"/>
-      <c r="D39" s="25"/>
-    </row>
-    <row r="40" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="22"/>
-      <c r="B40" s="30"/>
-      <c r="C40" s="23"/>
-      <c r="D40" s="25"/>
-    </row>
-    <row r="41" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="22"/>
-      <c r="B41" s="30"/>
-      <c r="C41" s="23"/>
-      <c r="D41" s="25"/>
-    </row>
-    <row r="42" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="22"/>
-      <c r="B42" s="30"/>
-      <c r="C42" s="23"/>
-      <c r="D42" s="25"/>
-    </row>
-    <row r="43" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="22"/>
-      <c r="B43" s="30"/>
-      <c r="C43" s="23"/>
-      <c r="D43" s="25"/>
-    </row>
-    <row r="44" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="22"/>
-      <c r="B44" s="30"/>
-      <c r="C44" s="23"/>
-      <c r="D44" s="25"/>
-    </row>
-    <row r="45" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="22"/>
-      <c r="B45" s="30"/>
-      <c r="C45" s="23"/>
-      <c r="D45" s="25"/>
-    </row>
-    <row r="46" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="22"/>
-      <c r="B46" s="30"/>
-      <c r="C46" s="23"/>
-      <c r="D46" s="24"/>
-    </row>
-    <row r="47" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="22"/>
-      <c r="B47" s="30"/>
-      <c r="C47" s="23"/>
-      <c r="D47" s="25"/>
-    </row>
-    <row r="48" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="22"/>
-      <c r="B48" s="30"/>
-      <c r="C48" s="23"/>
-      <c r="D48" s="25"/>
-    </row>
-    <row r="49" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="22"/>
-      <c r="B49" s="30"/>
-      <c r="C49" s="23"/>
-      <c r="D49" s="25"/>
-    </row>
-    <row r="50" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="22"/>
-      <c r="B50" s="30"/>
-      <c r="C50" s="23"/>
-      <c r="D50" s="25"/>
-    </row>
-    <row r="51" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="22"/>
-      <c r="B51" s="30"/>
-      <c r="C51" s="23"/>
-      <c r="D51" s="25"/>
-    </row>
-    <row r="52" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="22"/>
-      <c r="B52" s="30"/>
-      <c r="C52" s="23"/>
-      <c r="D52" s="25"/>
-    </row>
-    <row r="53" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="22"/>
-      <c r="B53" s="30"/>
-      <c r="C53" s="23"/>
-      <c r="D53" s="25"/>
-    </row>
-    <row r="54" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="26"/>
-      <c r="B54" s="31"/>
-      <c r="C54" s="27"/>
-      <c r="D54" s="28"/>
-    </row>
-    <row r="55" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="12"/>
-    </row>
-    <row r="56" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="12"/>
-    </row>
-    <row r="57" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="12"/>
-    </row>
-    <row r="58" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="12"/>
-    </row>
-    <row r="59" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="12"/>
-    </row>
-    <row r="60" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="12"/>
-    </row>
-    <row r="61" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="12"/>
-    </row>
-    <row r="62" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="12"/>
-    </row>
-    <row r="63" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="12"/>
-    </row>
-    <row r="64" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="12"/>
-    </row>
-    <row r="65" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="12"/>
-    </row>
-    <row r="66" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="12"/>
+      <c r="D3" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="21"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="23"/>
+    </row>
+    <row r="5" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="21"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="20"/>
+    </row>
+    <row r="6" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="21"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="24"/>
+    </row>
+    <row r="7" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="21"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="24"/>
+    </row>
+    <row r="8" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="21"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="23"/>
+    </row>
+    <row r="9" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="21"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="23"/>
+    </row>
+    <row r="10" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="21"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="23"/>
+    </row>
+    <row r="11" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="21"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="23"/>
+    </row>
+    <row r="12" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="21"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="23"/>
+    </row>
+    <row r="13" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="21"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="24"/>
+    </row>
+    <row r="14" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="21"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="24"/>
+    </row>
+    <row r="15" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="21"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="24"/>
+    </row>
+    <row r="16" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="21"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="24"/>
+    </row>
+    <row r="17" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="21"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="24"/>
+    </row>
+    <row r="18" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="21"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="24"/>
+    </row>
+    <row r="19" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="21"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="24"/>
+    </row>
+    <row r="20" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="21"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="24"/>
+    </row>
+    <row r="21" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="21"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="24"/>
+    </row>
+    <row r="22" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="21"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="24"/>
+    </row>
+    <row r="23" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="21"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="24"/>
+    </row>
+    <row r="24" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="21"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="24"/>
+    </row>
+    <row r="25" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="21"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="24"/>
+    </row>
+    <row r="26" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="21"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="24"/>
+    </row>
+    <row r="27" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="21"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="24"/>
+    </row>
+    <row r="28" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="21"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="24"/>
+    </row>
+    <row r="29" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="21"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="24"/>
+    </row>
+    <row r="30" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="21"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="24"/>
+    </row>
+    <row r="31" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="21"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="24"/>
+    </row>
+    <row r="32" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="21"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="24"/>
+    </row>
+    <row r="33" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="21"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="24"/>
+    </row>
+    <row r="34" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="21"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="24"/>
+    </row>
+    <row r="35" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="21"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="24"/>
+    </row>
+    <row r="36" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="21"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="23"/>
+    </row>
+    <row r="37" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="21"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="24"/>
+    </row>
+    <row r="38" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="21"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="24"/>
+    </row>
+    <row r="39" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="21"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="24"/>
+    </row>
+    <row r="40" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="21"/>
+      <c r="B40" s="29"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="24"/>
+    </row>
+    <row r="41" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="21"/>
+      <c r="B41" s="29"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="24"/>
+    </row>
+    <row r="42" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="21"/>
+      <c r="B42" s="29"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="24"/>
+    </row>
+    <row r="43" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="21"/>
+      <c r="B43" s="29"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="24"/>
+    </row>
+    <row r="44" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="21"/>
+      <c r="B44" s="29"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="24"/>
+    </row>
+    <row r="45" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="21"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="22"/>
+      <c r="D45" s="24"/>
+    </row>
+    <row r="46" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="21"/>
+      <c r="B46" s="29"/>
+      <c r="C46" s="22"/>
+      <c r="D46" s="23"/>
+    </row>
+    <row r="47" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="21"/>
+      <c r="B47" s="29"/>
+      <c r="C47" s="22"/>
+      <c r="D47" s="24"/>
+    </row>
+    <row r="48" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="21"/>
+      <c r="B48" s="29"/>
+      <c r="C48" s="22"/>
+      <c r="D48" s="24"/>
+    </row>
+    <row r="49" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="21"/>
+      <c r="B49" s="29"/>
+      <c r="C49" s="22"/>
+      <c r="D49" s="24"/>
+    </row>
+    <row r="50" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="21"/>
+      <c r="B50" s="29"/>
+      <c r="C50" s="22"/>
+      <c r="D50" s="24"/>
+    </row>
+    <row r="51" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="21"/>
+      <c r="B51" s="29"/>
+      <c r="C51" s="22"/>
+      <c r="D51" s="24"/>
+    </row>
+    <row r="52" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="21"/>
+      <c r="B52" s="29"/>
+      <c r="C52" s="22"/>
+      <c r="D52" s="24"/>
+    </row>
+    <row r="53" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="21"/>
+      <c r="B53" s="29"/>
+      <c r="C53" s="22"/>
+      <c r="D53" s="24"/>
+    </row>
+    <row r="54" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="25"/>
+      <c r="B54" s="30"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="27"/>
+    </row>
+    <row r="55" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="11"/>
+    </row>
+    <row r="56" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="11"/>
+    </row>
+    <row r="57" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="11"/>
+    </row>
+    <row r="58" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="11"/>
+    </row>
+    <row r="59" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="11"/>
+    </row>
+    <row r="60" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="11"/>
+    </row>
+    <row r="61" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="11"/>
+    </row>
+    <row r="62" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="11"/>
+    </row>
+    <row r="63" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="11"/>
+    </row>
+    <row r="64" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="11"/>
+    </row>
+    <row r="65" spans="1:1" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="11"/>
+    </row>
+    <row r="66" spans="1:1" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="11"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"WARNING"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Style"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"ERROR"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>